<commit_message>
Fix hard coded FY in link
</commit_message>
<xml_diff>
--- a/reference-files/figures-template.xlsx
+++ b/reference-files/figures-template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aliceb02\Desktop\end-of-life-pub\reference-files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\stats\irf\18-End-of-Life\Publication\RAP Development\end-of-life-pub\reference-files\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -29,6 +29,9 @@
     <sheet name="data" sheetId="18" r:id="rId15"/>
     <sheet name="calculation" sheetId="19" r:id="rId16"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId17"/>
+  </externalReferences>
   <definedNames>
     <definedName name="data_range">OFFSET(data!$A$2, 0, 0, calculation!$B$1, calculation!$B$2)</definedName>
     <definedName name="figure1_home">OFFSET('Figure 1 Background Data'!$C$8, 0, 0, calculation!$B$7, 1)</definedName>
@@ -1387,7 +1390,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -1436,7 +1438,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0" sourceLinked="0"/>
@@ -1452,7 +1453,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1692,7 +1692,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -1731,7 +1730,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0" sourceLinked="0"/>
@@ -1747,7 +1745,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1880,7 +1877,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -1919,7 +1915,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0" sourceLinked="0"/>
@@ -2115,7 +2110,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0" sourceLinked="0"/>
@@ -2445,7 +2439,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2547,7 +2540,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2628,7 +2620,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3681,6 +3672,52 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Notes"/>
+      <sheetName val="Figure 1"/>
+      <sheetName val="Figure 1 Background Data"/>
+      <sheetName val="Figure 2"/>
+      <sheetName val="Figure 2 Background Data"/>
+      <sheetName val="Figure 3"/>
+      <sheetName val="Figure 3 Background Data"/>
+      <sheetName val="Figure 4"/>
+      <sheetName val="Figure 4 Background Data"/>
+      <sheetName val="Figure 5"/>
+      <sheetName val="Figure 5 Background Data"/>
+      <sheetName val="Figure A3.1"/>
+      <sheetName val="Figure A3.1 Background Data"/>
+      <sheetName val="External Causes of Deaths"/>
+      <sheetName val="data"/>
+      <sheetName val="calculation"/>
+    </sheetNames>
+    <definedNames>
+      <definedName name="fy_max" refersTo="#REF!"/>
+    </definedNames>
+    <sheetDataSet>
+      <sheetData sheetId="0" refreshError="1"/>
+      <sheetData sheetId="1" refreshError="1"/>
+      <sheetData sheetId="2" refreshError="1"/>
+      <sheetData sheetId="3" refreshError="1"/>
+      <sheetData sheetId="4" refreshError="1"/>
+      <sheetData sheetId="5" refreshError="1"/>
+      <sheetData sheetId="6" refreshError="1"/>
+      <sheetData sheetId="7" refreshError="1"/>
+      <sheetData sheetId="8" refreshError="1"/>
+      <sheetData sheetId="9" refreshError="1"/>
+      <sheetData sheetId="10" refreshError="1"/>
+      <sheetData sheetId="11" refreshError="1"/>
+      <sheetData sheetId="12" refreshError="1"/>
+      <sheetData sheetId="13" refreshError="1"/>
+      <sheetData sheetId="14" refreshError="1"/>
+      <sheetData sheetId="15" refreshError="1"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -4315,7 +4352,7 @@
     <row r="6" spans="1:28" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="21"/>
       <c r="B6" s="11" t="e">
-        <f ca="1">"Figure 1: Percentage of time in the last six months of life spent at home or in a community setting; 2010/11 - " &amp; [0]!fy_max</f>
+        <f ca="1">"Figure 1: Percentage of time in the last six months of life spent at home or in a community setting; " &amp; calculation!B9 &amp; " - " &amp; [1]!fy_max</f>
         <v>#REF!</v>
       </c>
       <c r="C6" s="11"/>

</xml_diff>

<commit_message>
Updates to template excel output files to reflect manual changes made to publication.
</commit_message>
<xml_diff>
--- a/reference-files/figures-template.xlsx
+++ b/reference-files/figures-template.xlsx
@@ -373,9 +373,6 @@
     <t>Age Group</t>
   </si>
   <si>
-    <t>Gender</t>
-  </si>
-  <si>
     <t>0-54</t>
   </si>
   <si>
@@ -478,9 +475,6 @@
     <t>number of financial years</t>
   </si>
   <si>
-    <t>Health Board and Health and Social Care Partnership relate to location of residence at time of death. Health Board figures are based on the 2019 boundaries.</t>
-  </si>
-  <si>
     <t>For full details of the external causes of death which have been omitted, please click here.</t>
   </si>
   <si>
@@ -520,16 +514,7 @@
     <t>provisional note</t>
   </si>
   <si>
-    <t>Figures for the latest year should therefore be treated with caution as there could be an undercount of hospital admissions, particularly for people who died in the last three months of the year.  This is not expected to have a large impact on these published figures when they are revised in subsequent updates.</t>
-  </si>
-  <si>
     <t>provisional note (used by above)</t>
-  </si>
-  <si>
-    <t>2. The Health Board of Residence is the usual place of residence prior to death.</t>
-  </si>
-  <si>
-    <t>3. Health Boards are based on the NHS Board boundaries which came into effect 1st April 2014.</t>
   </si>
   <si>
     <t>http://www.who.int/classifications/icd/en/</t>
@@ -547,31 +532,46 @@
     <t>²</t>
   </si>
   <si>
-    <t>Figure 2: Percentage of time in the last six months of life spent at home or in a community setting; by Health Board of Residence</t>
-  </si>
-  <si>
-    <t>Figure 3: Percentage of time in the last six months of life spent at home or in a community setting; by Age and Gender</t>
-  </si>
-  <si>
     <t>Figure 4: Percentage of time in the last six months of life spent at home or in a community setting; by Deprivation Category</t>
   </si>
   <si>
     <t>Figure 5: Percentage of time in the last six months of life spent at home or in a community setting; by Urban/Rural Classification</t>
   </si>
   <si>
-    <t>Health Board of Residence</t>
+    <t>Figure 2: Percentage of time in the last six months of life spent at home or in a community setting; by NHS Board of Residence</t>
+  </si>
+  <si>
+    <t>Figure 3: Percentage of time in the last six months of life spent at home or in a community setting; by Age and Sex</t>
   </si>
   <si>
     <t>Health and Social Care Team, PHS</t>
   </si>
   <si>
+    <t>NHS Board relates to location of residence at time of death and is based on the 2019 boundaries.</t>
+  </si>
+  <si>
+    <t>2. The NHS Board of Residence is the usual place of residence prior to death.</t>
+  </si>
+  <si>
+    <t>3. NHS Boards are based on the NHS Board boundaries which came into effect 1st April 2014.</t>
+  </si>
+  <si>
+    <t>NHS Board of Residence</t>
+  </si>
+  <si>
+    <t>Sex</t>
+  </si>
+  <si>
     <t>2. Data are analysed by the 2020 ‘Scotland level’ Scottish Index of Multiple Deprivation (SIMD) population weighted quintiles. Each quintile consists of approximately 20% of the population living in Scotland, with deprivation quintile 1 indicating the population living in the most deprived areas.</t>
   </si>
   <si>
-    <t>p</t>
+    <t>ᴾ</t>
   </si>
   <si>
-    <t>Figure 1: Percentage of last six months of life spent at home or in a community setting Scotland; 2010/11 - 2019/20</t>
+    <t>See Appendix 2 of the full report for more information.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hospital activity data is estimated to be 96% complete at Scotland level. However this is much lower for Forth Valley (50%) and as a result estimated figures for 2019/20 have been calculated for NHS Forth Valley and the Health and Social Care Partnerships within this area. These estimates have also been included in the Scotland figure. </t>
   </si>
 </sst>
 </file>
@@ -581,7 +581,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="29" x14ac:knownFonts="1">
+  <fonts count="28" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -752,18 +752,10 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="11"/>
+      <sz val="10"/>
       <color rgb="FF3C4043"/>
       <name val="Arial"/>
       <family val="2"/>
-    </font>
-    <font>
-      <vertAlign val="superscript"/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="4">
@@ -866,7 +858,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="124">
+  <cellXfs count="123">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
@@ -998,12 +990,6 @@
     <xf numFmtId="49" fontId="20" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="4" fillId="2" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -1088,7 +1074,12 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="7" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="7" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="14">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1399,7 +1390,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -1448,7 +1438,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0" sourceLinked="0"/>
@@ -1464,7 +1453,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1704,7 +1692,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -1743,7 +1730,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0" sourceLinked="0"/>
@@ -1759,7 +1745,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1892,7 +1877,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -1931,7 +1915,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0" sourceLinked="0"/>
@@ -2127,7 +2110,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0" sourceLinked="0"/>
@@ -2457,7 +2439,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2559,7 +2540,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2640,7 +2620,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3989,216 +3968,216 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.6640625" style="91" customWidth="1"/>
-    <col min="2" max="2" width="3.44140625" style="91" customWidth="1"/>
-    <col min="3" max="256" width="9.109375" style="91"/>
-    <col min="257" max="257" width="1.6640625" style="91" customWidth="1"/>
-    <col min="258" max="258" width="3.44140625" style="91" customWidth="1"/>
-    <col min="259" max="512" width="9.109375" style="91"/>
-    <col min="513" max="513" width="1.6640625" style="91" customWidth="1"/>
-    <col min="514" max="514" width="3.44140625" style="91" customWidth="1"/>
-    <col min="515" max="768" width="9.109375" style="91"/>
-    <col min="769" max="769" width="1.6640625" style="91" customWidth="1"/>
-    <col min="770" max="770" width="3.44140625" style="91" customWidth="1"/>
-    <col min="771" max="1024" width="9.109375" style="91"/>
-    <col min="1025" max="1025" width="1.6640625" style="91" customWidth="1"/>
-    <col min="1026" max="1026" width="3.44140625" style="91" customWidth="1"/>
-    <col min="1027" max="1280" width="9.109375" style="91"/>
-    <col min="1281" max="1281" width="1.6640625" style="91" customWidth="1"/>
-    <col min="1282" max="1282" width="3.44140625" style="91" customWidth="1"/>
-    <col min="1283" max="1536" width="9.109375" style="91"/>
-    <col min="1537" max="1537" width="1.6640625" style="91" customWidth="1"/>
-    <col min="1538" max="1538" width="3.44140625" style="91" customWidth="1"/>
-    <col min="1539" max="1792" width="9.109375" style="91"/>
-    <col min="1793" max="1793" width="1.6640625" style="91" customWidth="1"/>
-    <col min="1794" max="1794" width="3.44140625" style="91" customWidth="1"/>
-    <col min="1795" max="2048" width="9.109375" style="91"/>
-    <col min="2049" max="2049" width="1.6640625" style="91" customWidth="1"/>
-    <col min="2050" max="2050" width="3.44140625" style="91" customWidth="1"/>
-    <col min="2051" max="2304" width="9.109375" style="91"/>
-    <col min="2305" max="2305" width="1.6640625" style="91" customWidth="1"/>
-    <col min="2306" max="2306" width="3.44140625" style="91" customWidth="1"/>
-    <col min="2307" max="2560" width="9.109375" style="91"/>
-    <col min="2561" max="2561" width="1.6640625" style="91" customWidth="1"/>
-    <col min="2562" max="2562" width="3.44140625" style="91" customWidth="1"/>
-    <col min="2563" max="2816" width="9.109375" style="91"/>
-    <col min="2817" max="2817" width="1.6640625" style="91" customWidth="1"/>
-    <col min="2818" max="2818" width="3.44140625" style="91" customWidth="1"/>
-    <col min="2819" max="3072" width="9.109375" style="91"/>
-    <col min="3073" max="3073" width="1.6640625" style="91" customWidth="1"/>
-    <col min="3074" max="3074" width="3.44140625" style="91" customWidth="1"/>
-    <col min="3075" max="3328" width="9.109375" style="91"/>
-    <col min="3329" max="3329" width="1.6640625" style="91" customWidth="1"/>
-    <col min="3330" max="3330" width="3.44140625" style="91" customWidth="1"/>
-    <col min="3331" max="3584" width="9.109375" style="91"/>
-    <col min="3585" max="3585" width="1.6640625" style="91" customWidth="1"/>
-    <col min="3586" max="3586" width="3.44140625" style="91" customWidth="1"/>
-    <col min="3587" max="3840" width="9.109375" style="91"/>
-    <col min="3841" max="3841" width="1.6640625" style="91" customWidth="1"/>
-    <col min="3842" max="3842" width="3.44140625" style="91" customWidth="1"/>
-    <col min="3843" max="4096" width="9.109375" style="91"/>
-    <col min="4097" max="4097" width="1.6640625" style="91" customWidth="1"/>
-    <col min="4098" max="4098" width="3.44140625" style="91" customWidth="1"/>
-    <col min="4099" max="4352" width="9.109375" style="91"/>
-    <col min="4353" max="4353" width="1.6640625" style="91" customWidth="1"/>
-    <col min="4354" max="4354" width="3.44140625" style="91" customWidth="1"/>
-    <col min="4355" max="4608" width="9.109375" style="91"/>
-    <col min="4609" max="4609" width="1.6640625" style="91" customWidth="1"/>
-    <col min="4610" max="4610" width="3.44140625" style="91" customWidth="1"/>
-    <col min="4611" max="4864" width="9.109375" style="91"/>
-    <col min="4865" max="4865" width="1.6640625" style="91" customWidth="1"/>
-    <col min="4866" max="4866" width="3.44140625" style="91" customWidth="1"/>
-    <col min="4867" max="5120" width="9.109375" style="91"/>
-    <col min="5121" max="5121" width="1.6640625" style="91" customWidth="1"/>
-    <col min="5122" max="5122" width="3.44140625" style="91" customWidth="1"/>
-    <col min="5123" max="5376" width="9.109375" style="91"/>
-    <col min="5377" max="5377" width="1.6640625" style="91" customWidth="1"/>
-    <col min="5378" max="5378" width="3.44140625" style="91" customWidth="1"/>
-    <col min="5379" max="5632" width="9.109375" style="91"/>
-    <col min="5633" max="5633" width="1.6640625" style="91" customWidth="1"/>
-    <col min="5634" max="5634" width="3.44140625" style="91" customWidth="1"/>
-    <col min="5635" max="5888" width="9.109375" style="91"/>
-    <col min="5889" max="5889" width="1.6640625" style="91" customWidth="1"/>
-    <col min="5890" max="5890" width="3.44140625" style="91" customWidth="1"/>
-    <col min="5891" max="6144" width="9.109375" style="91"/>
-    <col min="6145" max="6145" width="1.6640625" style="91" customWidth="1"/>
-    <col min="6146" max="6146" width="3.44140625" style="91" customWidth="1"/>
-    <col min="6147" max="6400" width="9.109375" style="91"/>
-    <col min="6401" max="6401" width="1.6640625" style="91" customWidth="1"/>
-    <col min="6402" max="6402" width="3.44140625" style="91" customWidth="1"/>
-    <col min="6403" max="6656" width="9.109375" style="91"/>
-    <col min="6657" max="6657" width="1.6640625" style="91" customWidth="1"/>
-    <col min="6658" max="6658" width="3.44140625" style="91" customWidth="1"/>
-    <col min="6659" max="6912" width="9.109375" style="91"/>
-    <col min="6913" max="6913" width="1.6640625" style="91" customWidth="1"/>
-    <col min="6914" max="6914" width="3.44140625" style="91" customWidth="1"/>
-    <col min="6915" max="7168" width="9.109375" style="91"/>
-    <col min="7169" max="7169" width="1.6640625" style="91" customWidth="1"/>
-    <col min="7170" max="7170" width="3.44140625" style="91" customWidth="1"/>
-    <col min="7171" max="7424" width="9.109375" style="91"/>
-    <col min="7425" max="7425" width="1.6640625" style="91" customWidth="1"/>
-    <col min="7426" max="7426" width="3.44140625" style="91" customWidth="1"/>
-    <col min="7427" max="7680" width="9.109375" style="91"/>
-    <col min="7681" max="7681" width="1.6640625" style="91" customWidth="1"/>
-    <col min="7682" max="7682" width="3.44140625" style="91" customWidth="1"/>
-    <col min="7683" max="7936" width="9.109375" style="91"/>
-    <col min="7937" max="7937" width="1.6640625" style="91" customWidth="1"/>
-    <col min="7938" max="7938" width="3.44140625" style="91" customWidth="1"/>
-    <col min="7939" max="8192" width="9.109375" style="91"/>
-    <col min="8193" max="8193" width="1.6640625" style="91" customWidth="1"/>
-    <col min="8194" max="8194" width="3.44140625" style="91" customWidth="1"/>
-    <col min="8195" max="8448" width="9.109375" style="91"/>
-    <col min="8449" max="8449" width="1.6640625" style="91" customWidth="1"/>
-    <col min="8450" max="8450" width="3.44140625" style="91" customWidth="1"/>
-    <col min="8451" max="8704" width="9.109375" style="91"/>
-    <col min="8705" max="8705" width="1.6640625" style="91" customWidth="1"/>
-    <col min="8706" max="8706" width="3.44140625" style="91" customWidth="1"/>
-    <col min="8707" max="8960" width="9.109375" style="91"/>
-    <col min="8961" max="8961" width="1.6640625" style="91" customWidth="1"/>
-    <col min="8962" max="8962" width="3.44140625" style="91" customWidth="1"/>
-    <col min="8963" max="9216" width="9.109375" style="91"/>
-    <col min="9217" max="9217" width="1.6640625" style="91" customWidth="1"/>
-    <col min="9218" max="9218" width="3.44140625" style="91" customWidth="1"/>
-    <col min="9219" max="9472" width="9.109375" style="91"/>
-    <col min="9473" max="9473" width="1.6640625" style="91" customWidth="1"/>
-    <col min="9474" max="9474" width="3.44140625" style="91" customWidth="1"/>
-    <col min="9475" max="9728" width="9.109375" style="91"/>
-    <col min="9729" max="9729" width="1.6640625" style="91" customWidth="1"/>
-    <col min="9730" max="9730" width="3.44140625" style="91" customWidth="1"/>
-    <col min="9731" max="9984" width="9.109375" style="91"/>
-    <col min="9985" max="9985" width="1.6640625" style="91" customWidth="1"/>
-    <col min="9986" max="9986" width="3.44140625" style="91" customWidth="1"/>
-    <col min="9987" max="10240" width="9.109375" style="91"/>
-    <col min="10241" max="10241" width="1.6640625" style="91" customWidth="1"/>
-    <col min="10242" max="10242" width="3.44140625" style="91" customWidth="1"/>
-    <col min="10243" max="10496" width="9.109375" style="91"/>
-    <col min="10497" max="10497" width="1.6640625" style="91" customWidth="1"/>
-    <col min="10498" max="10498" width="3.44140625" style="91" customWidth="1"/>
-    <col min="10499" max="10752" width="9.109375" style="91"/>
-    <col min="10753" max="10753" width="1.6640625" style="91" customWidth="1"/>
-    <col min="10754" max="10754" width="3.44140625" style="91" customWidth="1"/>
-    <col min="10755" max="11008" width="9.109375" style="91"/>
-    <col min="11009" max="11009" width="1.6640625" style="91" customWidth="1"/>
-    <col min="11010" max="11010" width="3.44140625" style="91" customWidth="1"/>
-    <col min="11011" max="11264" width="9.109375" style="91"/>
-    <col min="11265" max="11265" width="1.6640625" style="91" customWidth="1"/>
-    <col min="11266" max="11266" width="3.44140625" style="91" customWidth="1"/>
-    <col min="11267" max="11520" width="9.109375" style="91"/>
-    <col min="11521" max="11521" width="1.6640625" style="91" customWidth="1"/>
-    <col min="11522" max="11522" width="3.44140625" style="91" customWidth="1"/>
-    <col min="11523" max="11776" width="9.109375" style="91"/>
-    <col min="11777" max="11777" width="1.6640625" style="91" customWidth="1"/>
-    <col min="11778" max="11778" width="3.44140625" style="91" customWidth="1"/>
-    <col min="11779" max="12032" width="9.109375" style="91"/>
-    <col min="12033" max="12033" width="1.6640625" style="91" customWidth="1"/>
-    <col min="12034" max="12034" width="3.44140625" style="91" customWidth="1"/>
-    <col min="12035" max="12288" width="9.109375" style="91"/>
-    <col min="12289" max="12289" width="1.6640625" style="91" customWidth="1"/>
-    <col min="12290" max="12290" width="3.44140625" style="91" customWidth="1"/>
-    <col min="12291" max="12544" width="9.109375" style="91"/>
-    <col min="12545" max="12545" width="1.6640625" style="91" customWidth="1"/>
-    <col min="12546" max="12546" width="3.44140625" style="91" customWidth="1"/>
-    <col min="12547" max="12800" width="9.109375" style="91"/>
-    <col min="12801" max="12801" width="1.6640625" style="91" customWidth="1"/>
-    <col min="12802" max="12802" width="3.44140625" style="91" customWidth="1"/>
-    <col min="12803" max="13056" width="9.109375" style="91"/>
-    <col min="13057" max="13057" width="1.6640625" style="91" customWidth="1"/>
-    <col min="13058" max="13058" width="3.44140625" style="91" customWidth="1"/>
-    <col min="13059" max="13312" width="9.109375" style="91"/>
-    <col min="13313" max="13313" width="1.6640625" style="91" customWidth="1"/>
-    <col min="13314" max="13314" width="3.44140625" style="91" customWidth="1"/>
-    <col min="13315" max="13568" width="9.109375" style="91"/>
-    <col min="13569" max="13569" width="1.6640625" style="91" customWidth="1"/>
-    <col min="13570" max="13570" width="3.44140625" style="91" customWidth="1"/>
-    <col min="13571" max="13824" width="9.109375" style="91"/>
-    <col min="13825" max="13825" width="1.6640625" style="91" customWidth="1"/>
-    <col min="13826" max="13826" width="3.44140625" style="91" customWidth="1"/>
-    <col min="13827" max="14080" width="9.109375" style="91"/>
-    <col min="14081" max="14081" width="1.6640625" style="91" customWidth="1"/>
-    <col min="14082" max="14082" width="3.44140625" style="91" customWidth="1"/>
-    <col min="14083" max="14336" width="9.109375" style="91"/>
-    <col min="14337" max="14337" width="1.6640625" style="91" customWidth="1"/>
-    <col min="14338" max="14338" width="3.44140625" style="91" customWidth="1"/>
-    <col min="14339" max="14592" width="9.109375" style="91"/>
-    <col min="14593" max="14593" width="1.6640625" style="91" customWidth="1"/>
-    <col min="14594" max="14594" width="3.44140625" style="91" customWidth="1"/>
-    <col min="14595" max="14848" width="9.109375" style="91"/>
-    <col min="14849" max="14849" width="1.6640625" style="91" customWidth="1"/>
-    <col min="14850" max="14850" width="3.44140625" style="91" customWidth="1"/>
-    <col min="14851" max="15104" width="9.109375" style="91"/>
-    <col min="15105" max="15105" width="1.6640625" style="91" customWidth="1"/>
-    <col min="15106" max="15106" width="3.44140625" style="91" customWidth="1"/>
-    <col min="15107" max="15360" width="9.109375" style="91"/>
-    <col min="15361" max="15361" width="1.6640625" style="91" customWidth="1"/>
-    <col min="15362" max="15362" width="3.44140625" style="91" customWidth="1"/>
-    <col min="15363" max="15616" width="9.109375" style="91"/>
-    <col min="15617" max="15617" width="1.6640625" style="91" customWidth="1"/>
-    <col min="15618" max="15618" width="3.44140625" style="91" customWidth="1"/>
-    <col min="15619" max="15872" width="9.109375" style="91"/>
-    <col min="15873" max="15873" width="1.6640625" style="91" customWidth="1"/>
-    <col min="15874" max="15874" width="3.44140625" style="91" customWidth="1"/>
-    <col min="15875" max="16128" width="9.109375" style="91"/>
-    <col min="16129" max="16129" width="1.6640625" style="91" customWidth="1"/>
-    <col min="16130" max="16130" width="3.44140625" style="91" customWidth="1"/>
-    <col min="16131" max="16384" width="9.109375" style="91"/>
+    <col min="1" max="1" width="2.6640625" style="89" customWidth="1"/>
+    <col min="2" max="2" width="3.44140625" style="89" customWidth="1"/>
+    <col min="3" max="256" width="9.109375" style="89"/>
+    <col min="257" max="257" width="1.6640625" style="89" customWidth="1"/>
+    <col min="258" max="258" width="3.44140625" style="89" customWidth="1"/>
+    <col min="259" max="512" width="9.109375" style="89"/>
+    <col min="513" max="513" width="1.6640625" style="89" customWidth="1"/>
+    <col min="514" max="514" width="3.44140625" style="89" customWidth="1"/>
+    <col min="515" max="768" width="9.109375" style="89"/>
+    <col min="769" max="769" width="1.6640625" style="89" customWidth="1"/>
+    <col min="770" max="770" width="3.44140625" style="89" customWidth="1"/>
+    <col min="771" max="1024" width="9.109375" style="89"/>
+    <col min="1025" max="1025" width="1.6640625" style="89" customWidth="1"/>
+    <col min="1026" max="1026" width="3.44140625" style="89" customWidth="1"/>
+    <col min="1027" max="1280" width="9.109375" style="89"/>
+    <col min="1281" max="1281" width="1.6640625" style="89" customWidth="1"/>
+    <col min="1282" max="1282" width="3.44140625" style="89" customWidth="1"/>
+    <col min="1283" max="1536" width="9.109375" style="89"/>
+    <col min="1537" max="1537" width="1.6640625" style="89" customWidth="1"/>
+    <col min="1538" max="1538" width="3.44140625" style="89" customWidth="1"/>
+    <col min="1539" max="1792" width="9.109375" style="89"/>
+    <col min="1793" max="1793" width="1.6640625" style="89" customWidth="1"/>
+    <col min="1794" max="1794" width="3.44140625" style="89" customWidth="1"/>
+    <col min="1795" max="2048" width="9.109375" style="89"/>
+    <col min="2049" max="2049" width="1.6640625" style="89" customWidth="1"/>
+    <col min="2050" max="2050" width="3.44140625" style="89" customWidth="1"/>
+    <col min="2051" max="2304" width="9.109375" style="89"/>
+    <col min="2305" max="2305" width="1.6640625" style="89" customWidth="1"/>
+    <col min="2306" max="2306" width="3.44140625" style="89" customWidth="1"/>
+    <col min="2307" max="2560" width="9.109375" style="89"/>
+    <col min="2561" max="2561" width="1.6640625" style="89" customWidth="1"/>
+    <col min="2562" max="2562" width="3.44140625" style="89" customWidth="1"/>
+    <col min="2563" max="2816" width="9.109375" style="89"/>
+    <col min="2817" max="2817" width="1.6640625" style="89" customWidth="1"/>
+    <col min="2818" max="2818" width="3.44140625" style="89" customWidth="1"/>
+    <col min="2819" max="3072" width="9.109375" style="89"/>
+    <col min="3073" max="3073" width="1.6640625" style="89" customWidth="1"/>
+    <col min="3074" max="3074" width="3.44140625" style="89" customWidth="1"/>
+    <col min="3075" max="3328" width="9.109375" style="89"/>
+    <col min="3329" max="3329" width="1.6640625" style="89" customWidth="1"/>
+    <col min="3330" max="3330" width="3.44140625" style="89" customWidth="1"/>
+    <col min="3331" max="3584" width="9.109375" style="89"/>
+    <col min="3585" max="3585" width="1.6640625" style="89" customWidth="1"/>
+    <col min="3586" max="3586" width="3.44140625" style="89" customWidth="1"/>
+    <col min="3587" max="3840" width="9.109375" style="89"/>
+    <col min="3841" max="3841" width="1.6640625" style="89" customWidth="1"/>
+    <col min="3842" max="3842" width="3.44140625" style="89" customWidth="1"/>
+    <col min="3843" max="4096" width="9.109375" style="89"/>
+    <col min="4097" max="4097" width="1.6640625" style="89" customWidth="1"/>
+    <col min="4098" max="4098" width="3.44140625" style="89" customWidth="1"/>
+    <col min="4099" max="4352" width="9.109375" style="89"/>
+    <col min="4353" max="4353" width="1.6640625" style="89" customWidth="1"/>
+    <col min="4354" max="4354" width="3.44140625" style="89" customWidth="1"/>
+    <col min="4355" max="4608" width="9.109375" style="89"/>
+    <col min="4609" max="4609" width="1.6640625" style="89" customWidth="1"/>
+    <col min="4610" max="4610" width="3.44140625" style="89" customWidth="1"/>
+    <col min="4611" max="4864" width="9.109375" style="89"/>
+    <col min="4865" max="4865" width="1.6640625" style="89" customWidth="1"/>
+    <col min="4866" max="4866" width="3.44140625" style="89" customWidth="1"/>
+    <col min="4867" max="5120" width="9.109375" style="89"/>
+    <col min="5121" max="5121" width="1.6640625" style="89" customWidth="1"/>
+    <col min="5122" max="5122" width="3.44140625" style="89" customWidth="1"/>
+    <col min="5123" max="5376" width="9.109375" style="89"/>
+    <col min="5377" max="5377" width="1.6640625" style="89" customWidth="1"/>
+    <col min="5378" max="5378" width="3.44140625" style="89" customWidth="1"/>
+    <col min="5379" max="5632" width="9.109375" style="89"/>
+    <col min="5633" max="5633" width="1.6640625" style="89" customWidth="1"/>
+    <col min="5634" max="5634" width="3.44140625" style="89" customWidth="1"/>
+    <col min="5635" max="5888" width="9.109375" style="89"/>
+    <col min="5889" max="5889" width="1.6640625" style="89" customWidth="1"/>
+    <col min="5890" max="5890" width="3.44140625" style="89" customWidth="1"/>
+    <col min="5891" max="6144" width="9.109375" style="89"/>
+    <col min="6145" max="6145" width="1.6640625" style="89" customWidth="1"/>
+    <col min="6146" max="6146" width="3.44140625" style="89" customWidth="1"/>
+    <col min="6147" max="6400" width="9.109375" style="89"/>
+    <col min="6401" max="6401" width="1.6640625" style="89" customWidth="1"/>
+    <col min="6402" max="6402" width="3.44140625" style="89" customWidth="1"/>
+    <col min="6403" max="6656" width="9.109375" style="89"/>
+    <col min="6657" max="6657" width="1.6640625" style="89" customWidth="1"/>
+    <col min="6658" max="6658" width="3.44140625" style="89" customWidth="1"/>
+    <col min="6659" max="6912" width="9.109375" style="89"/>
+    <col min="6913" max="6913" width="1.6640625" style="89" customWidth="1"/>
+    <col min="6914" max="6914" width="3.44140625" style="89" customWidth="1"/>
+    <col min="6915" max="7168" width="9.109375" style="89"/>
+    <col min="7169" max="7169" width="1.6640625" style="89" customWidth="1"/>
+    <col min="7170" max="7170" width="3.44140625" style="89" customWidth="1"/>
+    <col min="7171" max="7424" width="9.109375" style="89"/>
+    <col min="7425" max="7425" width="1.6640625" style="89" customWidth="1"/>
+    <col min="7426" max="7426" width="3.44140625" style="89" customWidth="1"/>
+    <col min="7427" max="7680" width="9.109375" style="89"/>
+    <col min="7681" max="7681" width="1.6640625" style="89" customWidth="1"/>
+    <col min="7682" max="7682" width="3.44140625" style="89" customWidth="1"/>
+    <col min="7683" max="7936" width="9.109375" style="89"/>
+    <col min="7937" max="7937" width="1.6640625" style="89" customWidth="1"/>
+    <col min="7938" max="7938" width="3.44140625" style="89" customWidth="1"/>
+    <col min="7939" max="8192" width="9.109375" style="89"/>
+    <col min="8193" max="8193" width="1.6640625" style="89" customWidth="1"/>
+    <col min="8194" max="8194" width="3.44140625" style="89" customWidth="1"/>
+    <col min="8195" max="8448" width="9.109375" style="89"/>
+    <col min="8449" max="8449" width="1.6640625" style="89" customWidth="1"/>
+    <col min="8450" max="8450" width="3.44140625" style="89" customWidth="1"/>
+    <col min="8451" max="8704" width="9.109375" style="89"/>
+    <col min="8705" max="8705" width="1.6640625" style="89" customWidth="1"/>
+    <col min="8706" max="8706" width="3.44140625" style="89" customWidth="1"/>
+    <col min="8707" max="8960" width="9.109375" style="89"/>
+    <col min="8961" max="8961" width="1.6640625" style="89" customWidth="1"/>
+    <col min="8962" max="8962" width="3.44140625" style="89" customWidth="1"/>
+    <col min="8963" max="9216" width="9.109375" style="89"/>
+    <col min="9217" max="9217" width="1.6640625" style="89" customWidth="1"/>
+    <col min="9218" max="9218" width="3.44140625" style="89" customWidth="1"/>
+    <col min="9219" max="9472" width="9.109375" style="89"/>
+    <col min="9473" max="9473" width="1.6640625" style="89" customWidth="1"/>
+    <col min="9474" max="9474" width="3.44140625" style="89" customWidth="1"/>
+    <col min="9475" max="9728" width="9.109375" style="89"/>
+    <col min="9729" max="9729" width="1.6640625" style="89" customWidth="1"/>
+    <col min="9730" max="9730" width="3.44140625" style="89" customWidth="1"/>
+    <col min="9731" max="9984" width="9.109375" style="89"/>
+    <col min="9985" max="9985" width="1.6640625" style="89" customWidth="1"/>
+    <col min="9986" max="9986" width="3.44140625" style="89" customWidth="1"/>
+    <col min="9987" max="10240" width="9.109375" style="89"/>
+    <col min="10241" max="10241" width="1.6640625" style="89" customWidth="1"/>
+    <col min="10242" max="10242" width="3.44140625" style="89" customWidth="1"/>
+    <col min="10243" max="10496" width="9.109375" style="89"/>
+    <col min="10497" max="10497" width="1.6640625" style="89" customWidth="1"/>
+    <col min="10498" max="10498" width="3.44140625" style="89" customWidth="1"/>
+    <col min="10499" max="10752" width="9.109375" style="89"/>
+    <col min="10753" max="10753" width="1.6640625" style="89" customWidth="1"/>
+    <col min="10754" max="10754" width="3.44140625" style="89" customWidth="1"/>
+    <col min="10755" max="11008" width="9.109375" style="89"/>
+    <col min="11009" max="11009" width="1.6640625" style="89" customWidth="1"/>
+    <col min="11010" max="11010" width="3.44140625" style="89" customWidth="1"/>
+    <col min="11011" max="11264" width="9.109375" style="89"/>
+    <col min="11265" max="11265" width="1.6640625" style="89" customWidth="1"/>
+    <col min="11266" max="11266" width="3.44140625" style="89" customWidth="1"/>
+    <col min="11267" max="11520" width="9.109375" style="89"/>
+    <col min="11521" max="11521" width="1.6640625" style="89" customWidth="1"/>
+    <col min="11522" max="11522" width="3.44140625" style="89" customWidth="1"/>
+    <col min="11523" max="11776" width="9.109375" style="89"/>
+    <col min="11777" max="11777" width="1.6640625" style="89" customWidth="1"/>
+    <col min="11778" max="11778" width="3.44140625" style="89" customWidth="1"/>
+    <col min="11779" max="12032" width="9.109375" style="89"/>
+    <col min="12033" max="12033" width="1.6640625" style="89" customWidth="1"/>
+    <col min="12034" max="12034" width="3.44140625" style="89" customWidth="1"/>
+    <col min="12035" max="12288" width="9.109375" style="89"/>
+    <col min="12289" max="12289" width="1.6640625" style="89" customWidth="1"/>
+    <col min="12290" max="12290" width="3.44140625" style="89" customWidth="1"/>
+    <col min="12291" max="12544" width="9.109375" style="89"/>
+    <col min="12545" max="12545" width="1.6640625" style="89" customWidth="1"/>
+    <col min="12546" max="12546" width="3.44140625" style="89" customWidth="1"/>
+    <col min="12547" max="12800" width="9.109375" style="89"/>
+    <col min="12801" max="12801" width="1.6640625" style="89" customWidth="1"/>
+    <col min="12802" max="12802" width="3.44140625" style="89" customWidth="1"/>
+    <col min="12803" max="13056" width="9.109375" style="89"/>
+    <col min="13057" max="13057" width="1.6640625" style="89" customWidth="1"/>
+    <col min="13058" max="13058" width="3.44140625" style="89" customWidth="1"/>
+    <col min="13059" max="13312" width="9.109375" style="89"/>
+    <col min="13313" max="13313" width="1.6640625" style="89" customWidth="1"/>
+    <col min="13314" max="13314" width="3.44140625" style="89" customWidth="1"/>
+    <col min="13315" max="13568" width="9.109375" style="89"/>
+    <col min="13569" max="13569" width="1.6640625" style="89" customWidth="1"/>
+    <col min="13570" max="13570" width="3.44140625" style="89" customWidth="1"/>
+    <col min="13571" max="13824" width="9.109375" style="89"/>
+    <col min="13825" max="13825" width="1.6640625" style="89" customWidth="1"/>
+    <col min="13826" max="13826" width="3.44140625" style="89" customWidth="1"/>
+    <col min="13827" max="14080" width="9.109375" style="89"/>
+    <col min="14081" max="14081" width="1.6640625" style="89" customWidth="1"/>
+    <col min="14082" max="14082" width="3.44140625" style="89" customWidth="1"/>
+    <col min="14083" max="14336" width="9.109375" style="89"/>
+    <col min="14337" max="14337" width="1.6640625" style="89" customWidth="1"/>
+    <col min="14338" max="14338" width="3.44140625" style="89" customWidth="1"/>
+    <col min="14339" max="14592" width="9.109375" style="89"/>
+    <col min="14593" max="14593" width="1.6640625" style="89" customWidth="1"/>
+    <col min="14594" max="14594" width="3.44140625" style="89" customWidth="1"/>
+    <col min="14595" max="14848" width="9.109375" style="89"/>
+    <col min="14849" max="14849" width="1.6640625" style="89" customWidth="1"/>
+    <col min="14850" max="14850" width="3.44140625" style="89" customWidth="1"/>
+    <col min="14851" max="15104" width="9.109375" style="89"/>
+    <col min="15105" max="15105" width="1.6640625" style="89" customWidth="1"/>
+    <col min="15106" max="15106" width="3.44140625" style="89" customWidth="1"/>
+    <col min="15107" max="15360" width="9.109375" style="89"/>
+    <col min="15361" max="15361" width="1.6640625" style="89" customWidth="1"/>
+    <col min="15362" max="15362" width="3.44140625" style="89" customWidth="1"/>
+    <col min="15363" max="15616" width="9.109375" style="89"/>
+    <col min="15617" max="15617" width="1.6640625" style="89" customWidth="1"/>
+    <col min="15618" max="15618" width="3.44140625" style="89" customWidth="1"/>
+    <col min="15619" max="15872" width="9.109375" style="89"/>
+    <col min="15873" max="15873" width="1.6640625" style="89" customWidth="1"/>
+    <col min="15874" max="15874" width="3.44140625" style="89" customWidth="1"/>
+    <col min="15875" max="16128" width="9.109375" style="89"/>
+    <col min="16129" max="16129" width="1.6640625" style="89" customWidth="1"/>
+    <col min="16130" max="16130" width="3.44140625" style="89" customWidth="1"/>
+    <col min="16131" max="16384" width="9.109375" style="89"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:28" s="81" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A1" s="109"/>
-      <c r="B1" s="112"/>
-      <c r="C1" s="112"/>
-      <c r="D1" s="112"/>
-      <c r="E1" s="112"/>
-      <c r="F1" s="112"/>
-      <c r="G1" s="112"/>
-      <c r="H1" s="112"/>
-      <c r="I1" s="112"/>
-      <c r="J1" s="112"/>
-      <c r="K1" s="112"/>
-      <c r="L1" s="112"/>
-      <c r="M1" s="112"/>
-      <c r="N1" s="112"/>
-      <c r="O1" s="112"/>
+      <c r="A1" s="107"/>
+      <c r="B1" s="110"/>
+      <c r="C1" s="110"/>
+      <c r="D1" s="110"/>
+      <c r="E1" s="110"/>
+      <c r="F1" s="110"/>
+      <c r="G1" s="110"/>
+      <c r="H1" s="110"/>
+      <c r="I1" s="110"/>
+      <c r="J1" s="110"/>
+      <c r="K1" s="110"/>
+      <c r="L1" s="110"/>
+      <c r="M1" s="110"/>
+      <c r="N1" s="110"/>
+      <c r="O1" s="110"/>
     </row>
     <row r="2" spans="1:28" s="24" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="21"/>
@@ -4326,8 +4305,9 @@
     </row>
     <row r="6" spans="1:28" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="21"/>
-      <c r="B6" s="11" t="s">
-        <v>171</v>
+      <c r="B6" s="11" t="e">
+        <f ca="1">"Figure 1: Percentage of time in the last six months of life spent at home or in a community setting; " &amp; calculation!B9 &amp; " - " &amp; calculation!K9</f>
+        <v>#REF!</v>
       </c>
       <c r="C6" s="11"/>
       <c r="D6" s="11"/>
@@ -4359,7 +4339,7 @@
     <row r="7" spans="1:28" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="21"/>
       <c r="B7" s="11" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="C7" s="11"/>
       <c r="D7" s="11"/>
@@ -4391,7 +4371,7 @@
     <row r="8" spans="1:28" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="21"/>
       <c r="B8" s="11" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="C8" s="11"/>
       <c r="D8" s="11"/>
@@ -4423,7 +4403,7 @@
     <row r="9" spans="1:28" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="21"/>
       <c r="B9" s="11" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="C9" s="11"/>
       <c r="D9" s="11"/>
@@ -4455,7 +4435,7 @@
     <row r="10" spans="1:28" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="21"/>
       <c r="B10" s="11" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
       <c r="C10" s="11"/>
       <c r="D10" s="11"/>
@@ -4487,7 +4467,7 @@
     <row r="11" spans="1:28" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="21"/>
       <c r="B11" s="11" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C11" s="11"/>
       <c r="D11" s="11"/>
@@ -4581,7 +4561,7 @@
     <row r="14" spans="1:28" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="21"/>
       <c r="B14" s="24" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="C14" s="21"/>
       <c r="D14" s="21"/>
@@ -4707,23 +4687,23 @@
       <c r="B18" s="82" t="s">
         <v>74</v>
       </c>
-      <c r="C18" s="113" t="e">
+      <c r="C18" s="111" t="e">
         <f ca="1" xml:space="preserve"> calculation!B15</f>
         <v>#REF!</v>
       </c>
-      <c r="D18" s="114"/>
-      <c r="E18" s="114"/>
-      <c r="F18" s="114"/>
-      <c r="G18" s="114"/>
-      <c r="H18" s="114"/>
-      <c r="I18" s="114"/>
-      <c r="J18" s="114"/>
-      <c r="K18" s="114"/>
-      <c r="L18" s="114"/>
-      <c r="M18" s="114"/>
-      <c r="N18" s="114"/>
-      <c r="O18" s="114"/>
-      <c r="P18" s="114"/>
+      <c r="D18" s="112"/>
+      <c r="E18" s="112"/>
+      <c r="F18" s="112"/>
+      <c r="G18" s="112"/>
+      <c r="H18" s="112"/>
+      <c r="I18" s="112"/>
+      <c r="J18" s="112"/>
+      <c r="K18" s="112"/>
+      <c r="L18" s="112"/>
+      <c r="M18" s="112"/>
+      <c r="N18" s="112"/>
+      <c r="O18" s="112"/>
+      <c r="P18" s="112"/>
       <c r="Q18" s="21"/>
       <c r="R18" s="21"/>
       <c r="S18" s="21"/>
@@ -4740,20 +4720,22 @@
     <row r="19" spans="1:28" s="24" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A19" s="21"/>
       <c r="B19" s="82"/>
-      <c r="C19" s="83"/>
-      <c r="D19" s="84"/>
-      <c r="E19" s="84"/>
-      <c r="F19" s="84"/>
-      <c r="G19" s="84"/>
-      <c r="H19" s="84"/>
-      <c r="I19" s="84"/>
-      <c r="J19" s="84"/>
-      <c r="K19" s="84"/>
-      <c r="L19" s="84"/>
-      <c r="M19" s="84"/>
-      <c r="N19" s="84"/>
-      <c r="O19" s="84"/>
-      <c r="P19" s="84"/>
+      <c r="C19" s="122" t="s">
+        <v>170</v>
+      </c>
+      <c r="D19" s="122"/>
+      <c r="E19" s="122"/>
+      <c r="F19" s="122"/>
+      <c r="G19" s="122"/>
+      <c r="H19" s="122"/>
+      <c r="I19" s="122"/>
+      <c r="J19" s="122"/>
+      <c r="K19" s="122"/>
+      <c r="L19" s="122"/>
+      <c r="M19" s="122"/>
+      <c r="N19" s="122"/>
+      <c r="O19" s="122"/>
+      <c r="P19" s="122"/>
       <c r="Q19" s="21"/>
       <c r="R19" s="21"/>
       <c r="S19" s="21"/>
@@ -4798,28 +4780,28 @@
       <c r="AB20" s="21"/>
     </row>
     <row r="21" spans="1:28" s="21" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="85" t="s">
+      <c r="B21" s="83" t="s">
         <v>75</v>
       </c>
-      <c r="C21" s="111" t="s">
+      <c r="C21" s="109" t="s">
         <v>80</v>
       </c>
-      <c r="D21" s="111"/>
-      <c r="E21" s="111"/>
-      <c r="F21" s="111"/>
-      <c r="G21" s="111"/>
-      <c r="H21" s="111"/>
-      <c r="I21" s="111"/>
-      <c r="J21" s="111"/>
-      <c r="K21" s="111"/>
-      <c r="L21" s="111"/>
-      <c r="M21" s="111"/>
-      <c r="N21" s="111"/>
-      <c r="O21" s="111"/>
-      <c r="P21" s="111"/>
+      <c r="D21" s="109"/>
+      <c r="E21" s="109"/>
+      <c r="F21" s="109"/>
+      <c r="G21" s="109"/>
+      <c r="H21" s="109"/>
+      <c r="I21" s="109"/>
+      <c r="J21" s="109"/>
+      <c r="K21" s="109"/>
+      <c r="L21" s="109"/>
+      <c r="M21" s="109"/>
+      <c r="N21" s="109"/>
+      <c r="O21" s="109"/>
+      <c r="P21" s="109"/>
     </row>
     <row r="22" spans="1:28" s="21" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="85"/>
+      <c r="B22" s="83"/>
       <c r="C22" s="60"/>
       <c r="D22" s="60"/>
       <c r="E22" s="60"/>
@@ -4836,7 +4818,7 @@
       <c r="P22" s="60"/>
     </row>
     <row r="23" spans="1:28" s="21" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="85"/>
+      <c r="B23" s="83"/>
       <c r="C23" s="60"/>
       <c r="D23" s="60"/>
       <c r="E23" s="60"/>
@@ -4853,7 +4835,7 @@
       <c r="P23" s="60"/>
     </row>
     <row r="24" spans="1:28" s="21" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="85"/>
+      <c r="B24" s="83"/>
       <c r="C24" s="60"/>
       <c r="D24" s="60"/>
       <c r="E24" s="60"/>
@@ -4870,7 +4852,7 @@
       <c r="P24" s="60"/>
     </row>
     <row r="25" spans="1:28" s="21" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="85"/>
+      <c r="B25" s="83"/>
       <c r="C25" s="60"/>
       <c r="D25" s="60"/>
       <c r="E25" s="60"/>
@@ -4887,7 +4869,7 @@
       <c r="P25" s="60"/>
     </row>
     <row r="26" spans="1:28" s="21" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="85"/>
+      <c r="B26" s="83"/>
       <c r="C26" s="60"/>
       <c r="D26" s="60"/>
       <c r="E26" s="60"/>
@@ -4904,7 +4886,7 @@
       <c r="P26" s="60"/>
     </row>
     <row r="27" spans="1:28" s="21" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="85"/>
+      <c r="B27" s="83"/>
       <c r="C27" s="60"/>
       <c r="D27" s="60"/>
       <c r="E27" s="60"/>
@@ -4921,7 +4903,7 @@
       <c r="P27" s="60"/>
     </row>
     <row r="28" spans="1:28" s="21" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="85"/>
+      <c r="B28" s="83"/>
       <c r="C28" s="60"/>
       <c r="D28" s="60"/>
       <c r="E28" s="60"/>
@@ -4938,7 +4920,7 @@
       <c r="P28" s="60"/>
     </row>
     <row r="29" spans="1:28" s="21" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="85"/>
+      <c r="B29" s="83"/>
       <c r="C29" s="60"/>
       <c r="D29" s="60"/>
       <c r="E29" s="60"/>
@@ -4955,7 +4937,7 @@
       <c r="P29" s="60"/>
     </row>
     <row r="30" spans="1:28" s="21" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="85"/>
+      <c r="B30" s="83"/>
       <c r="C30" s="60"/>
       <c r="D30" s="60"/>
       <c r="E30" s="60"/>
@@ -4972,7 +4954,7 @@
       <c r="P30" s="60"/>
     </row>
     <row r="31" spans="1:28" s="21" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="85"/>
+      <c r="B31" s="83"/>
       <c r="C31" s="60"/>
       <c r="D31" s="60"/>
       <c r="E31" s="60"/>
@@ -4989,7 +4971,7 @@
       <c r="P31" s="60"/>
     </row>
     <row r="32" spans="1:28" s="21" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="85"/>
+      <c r="B32" s="83"/>
       <c r="C32" s="60"/>
       <c r="D32" s="60"/>
       <c r="E32" s="60"/>
@@ -5006,7 +4988,7 @@
       <c r="P32" s="60"/>
     </row>
     <row r="33" spans="2:16" s="21" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="85"/>
+      <c r="B33" s="83"/>
       <c r="C33" s="60"/>
       <c r="D33" s="60"/>
       <c r="E33" s="60"/>
@@ -5023,7 +5005,7 @@
       <c r="P33" s="60"/>
     </row>
     <row r="34" spans="2:16" s="21" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="85"/>
+      <c r="B34" s="83"/>
       <c r="C34" s="60"/>
       <c r="D34" s="60"/>
       <c r="E34" s="60"/>
@@ -5040,7 +5022,7 @@
       <c r="P34" s="60"/>
     </row>
     <row r="35" spans="2:16" s="21" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="85"/>
+      <c r="B35" s="83"/>
       <c r="C35" s="60"/>
       <c r="D35" s="60"/>
       <c r="E35" s="60"/>
@@ -5057,7 +5039,7 @@
       <c r="P35" s="60"/>
     </row>
     <row r="36" spans="2:16" s="21" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="85"/>
+      <c r="B36" s="83"/>
       <c r="C36" s="60"/>
       <c r="D36" s="60"/>
       <c r="E36" s="60"/>
@@ -5074,7 +5056,7 @@
       <c r="P36" s="60"/>
     </row>
     <row r="37" spans="2:16" s="21" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B37" s="85"/>
+      <c r="B37" s="83"/>
       <c r="C37" s="60"/>
       <c r="D37" s="60"/>
       <c r="E37" s="60"/>
@@ -5091,7 +5073,7 @@
       <c r="P37" s="60"/>
     </row>
     <row r="38" spans="2:16" s="21" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B38" s="85"/>
+      <c r="B38" s="83"/>
       <c r="C38" s="60"/>
       <c r="D38" s="60"/>
       <c r="E38" s="60"/>
@@ -5108,7 +5090,7 @@
       <c r="P38" s="60"/>
     </row>
     <row r="39" spans="2:16" s="21" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B39" s="85"/>
+      <c r="B39" s="83"/>
       <c r="C39" s="60"/>
       <c r="D39" s="60"/>
       <c r="E39" s="60"/>
@@ -5125,7 +5107,7 @@
       <c r="P39" s="60"/>
     </row>
     <row r="40" spans="2:16" s="21" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B40" s="85"/>
+      <c r="B40" s="83"/>
       <c r="C40" s="60"/>
       <c r="D40" s="60"/>
       <c r="E40" s="60"/>
@@ -5142,7 +5124,7 @@
       <c r="P40" s="60"/>
     </row>
     <row r="41" spans="2:16" s="21" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B41" s="85"/>
+      <c r="B41" s="83"/>
       <c r="C41" s="60"/>
       <c r="D41" s="60"/>
       <c r="E41" s="60"/>
@@ -5159,10 +5141,10 @@
       <c r="P41" s="60"/>
     </row>
     <row r="42" spans="2:16" s="21" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B42" s="85" t="s">
+      <c r="B42" s="83" t="s">
         <v>89</v>
       </c>
-      <c r="C42" s="86" t="s">
+      <c r="C42" s="84" t="s">
         <v>76</v>
       </c>
       <c r="D42" s="60"/>
@@ -5180,7 +5162,7 @@
       <c r="P42" s="60"/>
     </row>
     <row r="43" spans="2:16" s="21" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B43" s="85"/>
+      <c r="B43" s="83"/>
       <c r="C43" s="60"/>
       <c r="D43" s="60"/>
       <c r="E43" s="60"/>
@@ -5197,7 +5179,7 @@
       <c r="P43" s="60"/>
     </row>
     <row r="44" spans="2:16" s="21" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="B44" s="87" t="s">
+      <c r="B44" s="85" t="s">
         <v>85</v>
       </c>
       <c r="C44" s="21" t="s">
@@ -5205,9 +5187,9 @@
       </c>
     </row>
     <row r="45" spans="2:16" s="21" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="B45" s="88"/>
-      <c r="C45" s="89" t="s">
-        <v>141</v>
+      <c r="B45" s="86"/>
+      <c r="C45" s="87" t="s">
+        <v>139</v>
       </c>
       <c r="D45" s="74"/>
       <c r="E45" s="74"/>
@@ -5234,45 +5216,45 @@
       <c r="L46" s="28"/>
     </row>
     <row r="47" spans="2:16" s="21" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="B47" s="87"/>
+      <c r="B47" s="85"/>
     </row>
     <row r="48" spans="2:16" s="21" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="B48" s="88" t="s">
+      <c r="B48" s="86" t="s">
         <v>78</v>
       </c>
       <c r="C48" s="21" t="s">
-        <v>140</v>
+        <v>163</v>
       </c>
     </row>
     <row r="49" spans="1:16" s="21" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="B49" s="90"/>
+      <c r="B49" s="88"/>
       <c r="C49" s="60"/>
     </row>
     <row r="50" spans="1:16" s="21" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="85"/>
+      <c r="A50" s="83"/>
       <c r="B50" s="82" t="s">
         <v>90</v>
       </c>
-      <c r="C50" s="111" t="s">
+      <c r="C50" s="109" t="s">
         <v>82</v>
       </c>
-      <c r="D50" s="111"/>
-      <c r="E50" s="111"/>
-      <c r="F50" s="111"/>
-      <c r="G50" s="111"/>
-      <c r="H50" s="111"/>
-      <c r="I50" s="111"/>
-      <c r="J50" s="111"/>
-      <c r="K50" s="111"/>
-      <c r="L50" s="111"/>
-      <c r="M50" s="111"/>
-      <c r="N50" s="111"/>
-      <c r="O50" s="111"/>
-      <c r="P50" s="111"/>
+      <c r="D50" s="109"/>
+      <c r="E50" s="109"/>
+      <c r="F50" s="109"/>
+      <c r="G50" s="109"/>
+      <c r="H50" s="109"/>
+      <c r="I50" s="109"/>
+      <c r="J50" s="109"/>
+      <c r="K50" s="109"/>
+      <c r="L50" s="109"/>
+      <c r="M50" s="109"/>
+      <c r="N50" s="109"/>
+      <c r="O50" s="109"/>
+      <c r="P50" s="109"/>
     </row>
     <row r="51" spans="1:16" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="85"/>
-      <c r="B51" s="85"/>
+      <c r="A51" s="83"/>
+      <c r="B51" s="83"/>
     </row>
     <row r="52" spans="1:16" s="21" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="B52" s="82"/>
@@ -5300,11 +5282,12 @@
     <row r="73" s="21" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="74" s="21" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="5">
     <mergeCell ref="C21:P21"/>
     <mergeCell ref="C50:P50"/>
     <mergeCell ref="B1:O1"/>
     <mergeCell ref="C18:P18"/>
+    <mergeCell ref="C19:P19"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C45" location="'External Causes of Deaths'!A1" display="For full details of the external causes of death which have been omitted, please click here. "/>
@@ -5316,11 +5299,12 @@
     <hyperlink ref="B9" location="'Figure 4'!A1" display="Figure 4: Percentage of time in the last six months of life spent at home or in a community setting by Deprivation Category"/>
     <hyperlink ref="B10" location="'Figure 5'!A1" display="Figure 5: Percentage of time in the last six months of life spent at home or in a community setting (by Urban/Rural Classification)"/>
     <hyperlink ref="B11" location="'Figure A3.1'!A1" display="Figure A3.1: Percentage of time in the last six months of life spent at home or in a community setting; Comparison to old measure"/>
+    <hyperlink ref="C19" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.74803149606299213" right="0.74803149606299213" top="0.98425196850393704" bottom="0.98425196850393704" header="0.51181102362204722" footer="0.51181102362204722"/>
-  <pageSetup paperSize="9" scale="72" orientation="landscape" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="72" orientation="landscape" r:id="rId2"/>
   <headerFooter alignWithMargins="0"/>
-  <drawing r:id="rId2"/>
+  <drawing r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -5344,21 +5328,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:13" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B1" s="115"/>
-      <c r="C1" s="115"/>
-      <c r="D1" s="115"/>
-      <c r="E1" s="115"/>
-      <c r="F1" s="115"/>
-      <c r="G1" s="115"/>
-      <c r="H1" s="115"/>
-      <c r="I1" s="115"/>
-      <c r="J1" s="115"/>
-      <c r="K1" s="115"/>
-      <c r="L1" s="115"/>
+      <c r="B1" s="113"/>
+      <c r="C1" s="113"/>
+      <c r="D1" s="113"/>
+      <c r="E1" s="113"/>
+      <c r="F1" s="113"/>
+      <c r="G1" s="113"/>
+      <c r="H1" s="113"/>
+      <c r="I1" s="113"/>
+      <c r="J1" s="113"/>
+      <c r="K1" s="113"/>
+      <c r="L1" s="113"/>
     </row>
     <row r="2" spans="2:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B2" s="1" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
     </row>
     <row r="3" spans="2:13" ht="15.6" x14ac:dyDescent="0.3">
@@ -5368,7 +5352,7 @@
       </c>
     </row>
     <row r="4" spans="2:13" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="M4" s="100" t="e">
+      <c r="M4" s="98" t="e">
         <f ca="1" xml:space="preserve"> "Financial year ending 31st March 20" &amp; RIGHT([0]!fy_max, 2)</f>
         <v>#REF!</v>
       </c>
@@ -5383,7 +5367,7 @@
       <c r="F31" s="74"/>
     </row>
     <row r="32" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B32" s="101"/>
+      <c r="B32" s="99"/>
     </row>
     <row r="33" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B33" s="3" t="s">
@@ -5392,7 +5376,7 @@
     </row>
     <row r="34" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B34" s="4" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
     </row>
     <row r="35" spans="2:7" x14ac:dyDescent="0.25">
@@ -5403,10 +5387,10 @@
     </row>
     <row r="36" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B36" s="58" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="G36" s="33" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
   </sheetData>
@@ -5448,19 +5432,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:19" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B1" s="115"/>
-      <c r="C1" s="115"/>
-      <c r="D1" s="115"/>
-      <c r="E1" s="115"/>
-      <c r="F1" s="115"/>
-      <c r="G1" s="115"/>
-      <c r="H1" s="115"/>
-      <c r="I1" s="115"/>
-      <c r="J1" s="115"/>
-      <c r="K1" s="115"/>
-      <c r="L1" s="115"/>
-      <c r="M1" s="115"/>
-      <c r="N1" s="115"/>
+      <c r="B1" s="113"/>
+      <c r="C1" s="113"/>
+      <c r="D1" s="113"/>
+      <c r="E1" s="113"/>
+      <c r="F1" s="113"/>
+      <c r="G1" s="113"/>
+      <c r="H1" s="113"/>
+      <c r="I1" s="113"/>
+      <c r="J1" s="113"/>
+      <c r="K1" s="113"/>
+      <c r="L1" s="113"/>
+      <c r="M1" s="113"/>
+      <c r="N1" s="113"/>
       <c r="O1" s="66"/>
       <c r="P1" s="66"/>
       <c r="Q1" s="66"/>
@@ -5469,7 +5453,7 @@
     </row>
     <row r="2" spans="2:19" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B2" s="1" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
@@ -5494,7 +5478,7 @@
     </row>
     <row r="6" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B6" s="52" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C6" s="43" t="e">
         <f ca="1">CONCATENATE([0]!fy_max, calculation!$B$4)</f>
@@ -5503,7 +5487,7 @@
     </row>
     <row r="7" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B7" s="45" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C7" s="53" t="e">
         <f ca="1">VLOOKUP(CONCATENATE([0]!fy_max, "urban rural 6", $B7), [0]!data_range, 5, FALSE)</f>
@@ -5512,7 +5496,7 @@
     </row>
     <row r="8" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B8" s="47" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C8" s="54" t="e">
         <f ca="1">VLOOKUP(CONCATENATE([0]!fy_max, "urban rural 6", $B8), [0]!data_range, 5, FALSE)</f>
@@ -5521,7 +5505,7 @@
     </row>
     <row r="9" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B9" s="47" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C9" s="54" t="e">
         <f ca="1">VLOOKUP(CONCATENATE([0]!fy_max, "urban rural 6", $B9), [0]!data_range, 5, FALSE)</f>
@@ -5530,7 +5514,7 @@
     </row>
     <row r="10" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B10" s="47" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C10" s="54" t="e">
         <f ca="1">VLOOKUP(CONCATENATE([0]!fy_max, "urban rural 6", $B10), [0]!data_range, 5, FALSE)</f>
@@ -5539,7 +5523,7 @@
     </row>
     <row r="11" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B11" s="47" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C11" s="54" t="e">
         <f ca="1">VLOOKUP(CONCATENATE([0]!fy_max, "urban rural 6", $B11), [0]!data_range, 5, FALSE)</f>
@@ -5548,7 +5532,7 @@
     </row>
     <row r="12" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B12" s="49" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C12" s="55" t="e">
         <f ca="1">VLOOKUP(CONCATENATE([0]!fy_max, "urban rural 6", $B12), [0]!data_range, 5, FALSE)</f>
@@ -5569,14 +5553,14 @@
       <c r="J14" s="74"/>
     </row>
     <row r="15" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B15" s="101"/>
-      <c r="C15" s="101"/>
-      <c r="D15" s="101"/>
-      <c r="E15" s="101"/>
-      <c r="F15" s="101"/>
-      <c r="G15" s="101"/>
-      <c r="H15" s="101"/>
-      <c r="I15" s="101"/>
+      <c r="B15" s="99"/>
+      <c r="C15" s="99"/>
+      <c r="D15" s="99"/>
+      <c r="E15" s="99"/>
+      <c r="F15" s="99"/>
+      <c r="G15" s="99"/>
+      <c r="H15" s="99"/>
+      <c r="I15" s="99"/>
     </row>
     <row r="16" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B16" s="3" t="s">
@@ -5592,7 +5576,7 @@
     </row>
     <row r="17" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B17" s="4" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="C17" s="4"/>
       <c r="D17" s="4"/>
@@ -5610,10 +5594,10 @@
     </row>
     <row r="19" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B19" s="58" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D19" s="33" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
   </sheetData>
@@ -5648,21 +5632,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B1" s="115"/>
-      <c r="C1" s="115"/>
-      <c r="D1" s="115"/>
-      <c r="E1" s="115"/>
-      <c r="F1" s="115"/>
-      <c r="G1" s="115"/>
-      <c r="H1" s="115"/>
-      <c r="I1" s="115"/>
-      <c r="J1" s="115"/>
-      <c r="K1" s="115"/>
-      <c r="L1" s="115"/>
+      <c r="B1" s="113"/>
+      <c r="C1" s="113"/>
+      <c r="D1" s="113"/>
+      <c r="E1" s="113"/>
+      <c r="F1" s="113"/>
+      <c r="G1" s="113"/>
+      <c r="H1" s="113"/>
+      <c r="I1" s="113"/>
+      <c r="J1" s="113"/>
+      <c r="K1" s="113"/>
+      <c r="L1" s="113"/>
     </row>
     <row r="2" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B2" s="1" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="3" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
@@ -5672,7 +5656,7 @@
       </c>
     </row>
     <row r="4" spans="2:12" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="J4" s="92"/>
+      <c r="J4" s="90"/>
     </row>
     <row r="26" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B26" s="11" t="s">
@@ -5693,7 +5677,7 @@
     </row>
     <row r="29" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B29" s="4" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
     </row>
     <row r="30" spans="2:6" x14ac:dyDescent="0.25">
@@ -5727,29 +5711,29 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.6640625" style="93" customWidth="1"/>
-    <col min="2" max="2" width="14.88671875" style="95" customWidth="1"/>
-    <col min="3" max="3" width="17.44140625" style="95" customWidth="1"/>
-    <col min="4" max="4" width="25.109375" style="95" customWidth="1"/>
-    <col min="5" max="16384" width="9.109375" style="95"/>
+    <col min="1" max="1" width="2.6640625" style="91" customWidth="1"/>
+    <col min="2" max="2" width="14.88671875" style="93" customWidth="1"/>
+    <col min="3" max="3" width="17.44140625" style="93" customWidth="1"/>
+    <col min="4" max="4" width="25.109375" style="93" customWidth="1"/>
+    <col min="5" max="16384" width="9.109375" style="93"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B1" s="117"/>
-      <c r="C1" s="117"/>
-      <c r="D1" s="117"/>
-      <c r="E1" s="117"/>
-      <c r="F1" s="117"/>
-      <c r="G1" s="117"/>
-      <c r="H1" s="117"/>
-      <c r="I1" s="94"/>
-      <c r="J1" s="94"/>
-      <c r="K1" s="94"/>
-      <c r="L1" s="94"/>
+      <c r="B1" s="115"/>
+      <c r="C1" s="115"/>
+      <c r="D1" s="115"/>
+      <c r="E1" s="115"/>
+      <c r="F1" s="115"/>
+      <c r="G1" s="115"/>
+      <c r="H1" s="115"/>
+      <c r="I1" s="92"/>
+      <c r="J1" s="92"/>
+      <c r="K1" s="92"/>
+      <c r="L1" s="92"/>
     </row>
     <row r="2" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B2" s="1" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
@@ -5759,25 +5743,25 @@
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B5" s="96"/>
+      <c r="B5" s="94"/>
       <c r="F5" s="29"/>
     </row>
     <row r="6" spans="1:12" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="B6" s="108" t="s">
+      <c r="B6" s="106" t="s">
         <v>83</v>
       </c>
       <c r="C6" s="43" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="D6" s="59" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="E6" s="29"/>
       <c r="F6" s="29"/>
       <c r="G6" s="29"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" s="93" t="e">
+      <c r="A7" s="91" t="e">
         <f t="array" aca="1" ref="A7" ca="1">INDEX(fy_range, MATCH(0, COUNTIF($A$6:A6, fy_range), 0))</f>
         <v>#REF!</v>
       </c>
@@ -5794,11 +5778,11 @@
         <v>#REF!</v>
       </c>
       <c r="E7" s="29"/>
-      <c r="F7" s="98"/>
-      <c r="G7" s="98"/>
+      <c r="F7" s="96"/>
+      <c r="G7" s="96"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" s="93" t="e">
+      <c r="A8" s="91" t="e">
         <f t="array" aca="1" ref="A8" ca="1">INDEX(fy_range, MATCH(0, COUNTIF($A$6:A7, fy_range), 0))</f>
         <v>#REF!</v>
       </c>
@@ -5815,12 +5799,12 @@
         <v>#REF!</v>
       </c>
       <c r="E8" s="29"/>
-      <c r="F8" s="98"/>
-      <c r="G8" s="98"/>
-      <c r="I8" s="98"/>
+      <c r="F8" s="96"/>
+      <c r="G8" s="96"/>
+      <c r="I8" s="96"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" s="93" t="e">
+      <c r="A9" s="91" t="e">
         <f t="array" aca="1" ref="A9" ca="1">INDEX(fy_range, MATCH(0, COUNTIF($A$6:A8, fy_range), 0))</f>
         <v>#REF!</v>
       </c>
@@ -5837,12 +5821,12 @@
         <v>#REF!</v>
       </c>
       <c r="E9" s="29"/>
-      <c r="F9" s="98"/>
-      <c r="G9" s="98"/>
-      <c r="I9" s="98"/>
+      <c r="F9" s="96"/>
+      <c r="G9" s="96"/>
+      <c r="I9" s="96"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" s="93" t="e">
+      <c r="A10" s="91" t="e">
         <f t="array" aca="1" ref="A10" ca="1">INDEX(fy_range, MATCH(0, COUNTIF($A$6:A9, fy_range), 0))</f>
         <v>#REF!</v>
       </c>
@@ -5859,12 +5843,12 @@
         <v>#REF!</v>
       </c>
       <c r="E10" s="29"/>
-      <c r="F10" s="98"/>
-      <c r="G10" s="98"/>
-      <c r="I10" s="98"/>
+      <c r="F10" s="96"/>
+      <c r="G10" s="96"/>
+      <c r="I10" s="96"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" s="93" t="e">
+      <c r="A11" s="91" t="e">
         <f t="array" aca="1" ref="A11" ca="1">INDEX(fy_range, MATCH(0, COUNTIF($A$6:A10, fy_range), 0))</f>
         <v>#REF!</v>
       </c>
@@ -5881,13 +5865,13 @@
         <v>#REF!</v>
       </c>
       <c r="E11" s="29"/>
-      <c r="F11" s="98"/>
-      <c r="G11" s="98"/>
-      <c r="I11" s="98"/>
-      <c r="J11" s="96"/>
+      <c r="F11" s="96"/>
+      <c r="G11" s="96"/>
+      <c r="I11" s="96"/>
+      <c r="J11" s="94"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A12" s="93" t="e">
+      <c r="A12" s="91" t="e">
         <f t="array" aca="1" ref="A12" ca="1">INDEX(fy_range, MATCH(0, COUNTIF($A$6:A11, fy_range), 0))</f>
         <v>#REF!</v>
       </c>
@@ -5904,13 +5888,13 @@
         <v>#REF!</v>
       </c>
       <c r="E12" s="32"/>
-      <c r="F12" s="98"/>
-      <c r="G12" s="98"/>
-      <c r="I12" s="98"/>
-      <c r="J12" s="96"/>
+      <c r="F12" s="96"/>
+      <c r="G12" s="96"/>
+      <c r="I12" s="96"/>
+      <c r="J12" s="94"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A13" s="93" t="e">
+      <c r="A13" s="91" t="e">
         <f t="array" aca="1" ref="A13" ca="1">INDEX(fy_range, MATCH(0, COUNTIF($A$6:A12, fy_range), 0))</f>
         <v>#REF!</v>
       </c>
@@ -5927,13 +5911,13 @@
         <v>#REF!</v>
       </c>
       <c r="E13" s="32"/>
-      <c r="F13" s="98"/>
-      <c r="G13" s="98"/>
-      <c r="I13" s="98"/>
-      <c r="J13" s="96"/>
+      <c r="F13" s="96"/>
+      <c r="G13" s="96"/>
+      <c r="I13" s="96"/>
+      <c r="J13" s="94"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A14" s="93" t="e">
+      <c r="A14" s="91" t="e">
         <f t="array" aca="1" ref="A14" ca="1">INDEX(fy_range, MATCH(0, COUNTIF($A$6:A13, fy_range), 0))</f>
         <v>#REF!</v>
       </c>
@@ -5950,13 +5934,13 @@
         <v>#REF!</v>
       </c>
       <c r="E14" s="32"/>
-      <c r="F14" s="98"/>
-      <c r="G14" s="98"/>
-      <c r="I14" s="98"/>
-      <c r="J14" s="96"/>
+      <c r="F14" s="96"/>
+      <c r="G14" s="96"/>
+      <c r="I14" s="96"/>
+      <c r="J14" s="94"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A15" s="99" t="e">
+      <c r="A15" s="97" t="e">
         <f t="array" aca="1" ref="A15" ca="1">INDEX(fy_range, MATCH(0, COUNTIF($A$6:A14, fy_range), 0))</f>
         <v>#REF!</v>
       </c>
@@ -5973,11 +5957,11 @@
         <v>#REF!</v>
       </c>
       <c r="E15" s="32"/>
-      <c r="I15" s="98"/>
-      <c r="J15" s="96"/>
+      <c r="I15" s="96"/>
+      <c r="J15" s="94"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A16" s="99" t="e">
+      <c r="A16" s="97" t="e">
         <f t="array" aca="1" ref="A16" ca="1">INDEX(fy_range, MATCH(0, COUNTIF($A$6:A15, fy_range), 0))</f>
         <v>#REF!</v>
       </c>
@@ -5996,20 +5980,20 @@
       <c r="E16" s="29"/>
       <c r="F16" s="29"/>
       <c r="G16" s="29"/>
-      <c r="H16" s="96"/>
-      <c r="I16" s="96"/>
-      <c r="J16" s="96"/>
+      <c r="H16" s="94"/>
+      <c r="I16" s="94"/>
+      <c r="J16" s="94"/>
     </row>
     <row r="17" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B17" s="96"/>
+      <c r="B17" s="94"/>
       <c r="C17" s="29"/>
       <c r="D17" s="29"/>
       <c r="E17" s="29"/>
       <c r="F17" s="29"/>
       <c r="G17" s="29"/>
-      <c r="H17" s="96"/>
-      <c r="I17" s="96"/>
-      <c r="J17" s="96"/>
+      <c r="H17" s="94"/>
+      <c r="I17" s="94"/>
+      <c r="J17" s="94"/>
     </row>
     <row r="18" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B18" s="11" t="s">
@@ -6028,7 +6012,7 @@
     </row>
     <row r="21" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B21" s="4" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
     </row>
     <row r="22" spans="2:10" x14ac:dyDescent="0.25">
@@ -6666,10 +6650,10 @@
     </row>
     <row r="20" spans="1:4" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="30"/>
-      <c r="B20" s="120" t="s">
+      <c r="B20" s="118" t="s">
         <v>28</v>
       </c>
-      <c r="C20" s="120"/>
+      <c r="C20" s="118"/>
       <c r="D20" s="13"/>
     </row>
     <row r="21" spans="1:4" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -6834,16 +6818,16 @@
     </row>
     <row r="37" spans="1:4" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="30"/>
-      <c r="B37" s="121"/>
-      <c r="C37" s="121"/>
+      <c r="B37" s="119"/>
+      <c r="C37" s="119"/>
       <c r="D37" s="13"/>
     </row>
     <row r="38" spans="1:4" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="30"/>
-      <c r="B38" s="120" t="s">
+      <c r="B38" s="118" t="s">
         <v>61</v>
       </c>
-      <c r="C38" s="120"/>
+      <c r="C38" s="118"/>
       <c r="D38" s="13"/>
     </row>
     <row r="39" spans="1:4" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -6911,7 +6895,7 @@
     <row r="47" spans="1:4" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="30"/>
       <c r="B47" s="5" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="C47" s="2"/>
       <c r="D47" s="13"/>
@@ -7863,22 +7847,22 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="34" t="s">
+        <v>118</v>
+      </c>
+      <c r="B1" s="34" t="s">
         <v>119</v>
       </c>
-      <c r="B1" s="34" t="s">
+      <c r="C1" s="34" t="s">
         <v>120</v>
       </c>
-      <c r="C1" s="34" t="s">
+      <c r="D1" s="34" t="s">
         <v>121</v>
       </c>
-      <c r="D1" s="34" t="s">
+      <c r="E1" s="34" t="s">
         <v>122</v>
       </c>
-      <c r="E1" s="34" t="s">
+      <c r="F1" s="34" t="s">
         <v>123</v>
-      </c>
-      <c r="F1" s="34" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -30021,7 +30005,7 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="38" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B1" s="39">
         <f>COUNTA(data!B:B)-1</f>
@@ -30030,42 +30014,42 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="38" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B2" s="39">
         <f>COUNTA(data!1:1)</f>
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="38" t="s">
-        <v>135</v>
-      </c>
-      <c r="B4" s="123" t="s">
-        <v>170</v>
+        <v>134</v>
+      </c>
+      <c r="B4" s="56" t="s">
+        <v>169</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="38" t="s">
+        <v>136</v>
+      </c>
+      <c r="B5" s="39" t="s">
         <v>137</v>
       </c>
-      <c r="B5" s="39" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" ht="13.8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="38" t="s">
-        <v>161</v>
-      </c>
-      <c r="B6" s="110" t="s">
-        <v>162</v>
+        <v>156</v>
+      </c>
+      <c r="B6" s="108" t="s">
+        <v>157</v>
       </c>
       <c r="I6" s="38"/>
       <c r="K6" s="38"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="38" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B7" s="39">
         <v>10</v>
@@ -30176,56 +30160,64 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="38" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B13" s="38" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="38" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B14" s="39" t="e">
-        <f ca="1">"Data for "&amp; $K$9 &amp;" are provisional" &amp; IF($B$13="provisional"," and will be revised in October 20"&amp;RIGHT($K$9,2)&amp;" publication.", ".")</f>
+        <f ca="1">"Data for "&amp; $K$9 &amp;" are provisional. Please see Notes tab for more information."</f>
         <v>#REF!</v>
       </c>
     </row>
     <row r="15" spans="1:11" ht="80.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="61" t="s">
-        <v>153</v>
-      </c>
-      <c r="B15" s="122" t="e">
-        <f ca="1">IF($B$13 = "provisional", "Hospital data and ", "") &amp; "National Records of Scotland deaths data " &amp; IF($B$13 = "provisional", "are", "is") &amp; " provisional for " &amp; $K$9 &amp;". " &amp; IF($B$13 = "provisional", "This publication will be updated in October 20" &amp; RIGHT($K$9,2) &amp; " with final figures. " &amp; $B$16, "")</f>
+        <v>151</v>
+      </c>
+      <c r="B15" s="120" t="e">
+        <f ca="1">IF($B$13 = "provisional", "Hospital data and ", "") &amp; "National Records of Scotland deaths data " &amp; IF($B$13 = "provisional", "are", "is") &amp; " provisional for " &amp; $K$9 &amp;". " &amp; IF($B$13 = "provisional", "This publication will be updated in October 20" &amp; RIGHT($K$9,2) &amp; ". " &amp; $B$16, "")</f>
         <v>#REF!</v>
       </c>
-      <c r="C15" s="122"/>
-      <c r="D15" s="122"/>
-      <c r="E15" s="122"/>
-      <c r="F15" s="122"/>
-      <c r="G15" s="122"/>
-      <c r="H15" s="122"/>
-      <c r="I15" s="122"/>
+      <c r="C15" s="120"/>
+      <c r="D15" s="120"/>
+      <c r="E15" s="120"/>
+      <c r="F15" s="120"/>
+      <c r="G15" s="120"/>
+      <c r="H15" s="120"/>
+      <c r="I15" s="120"/>
     </row>
     <row r="16" spans="1:11" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="38" t="s">
-        <v>155</v>
-      </c>
-      <c r="B16" s="122" t="s">
-        <v>154</v>
-      </c>
-      <c r="C16" s="122"/>
-      <c r="D16" s="122"/>
-      <c r="E16" s="122"/>
-      <c r="F16" s="122"/>
-      <c r="G16" s="122"/>
-      <c r="H16" s="122"/>
-      <c r="I16" s="122"/>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+        <v>152</v>
+      </c>
+      <c r="B16" s="121" t="s">
+        <v>171</v>
+      </c>
+      <c r="C16" s="120"/>
+      <c r="D16" s="120"/>
+      <c r="E16" s="120"/>
+      <c r="F16" s="120"/>
+      <c r="G16" s="120"/>
+      <c r="H16" s="120"/>
+      <c r="I16" s="120"/>
+    </row>
+    <row r="17" spans="1:9" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="38"/>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B17" s="2"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+      <c r="G17" s="2"/>
+      <c r="H17" s="2"/>
+      <c r="I17" s="2"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="38"/>
       <c r="B18" s="62"/>
       <c r="C18" s="63"/>
@@ -30235,22 +30227,22 @@
       <c r="G18" s="63"/>
       <c r="H18" s="63"/>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="38"/>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="38"/>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="38"/>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="38"/>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="38"/>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="38"/>
     </row>
   </sheetData>
@@ -30281,17 +30273,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B1" s="115"/>
-      <c r="C1" s="115"/>
-      <c r="D1" s="115"/>
-      <c r="E1" s="115"/>
-      <c r="F1" s="115"/>
-      <c r="G1" s="115"/>
-      <c r="H1" s="115"/>
-      <c r="I1" s="115"/>
-      <c r="J1" s="115"/>
-      <c r="K1" s="115"/>
-      <c r="L1" s="115"/>
+      <c r="B1" s="113"/>
+      <c r="C1" s="113"/>
+      <c r="D1" s="113"/>
+      <c r="E1" s="113"/>
+      <c r="F1" s="113"/>
+      <c r="G1" s="113"/>
+      <c r="H1" s="113"/>
+      <c r="I1" s="113"/>
+      <c r="J1" s="113"/>
+      <c r="K1" s="113"/>
+      <c r="L1" s="113"/>
     </row>
     <row r="2" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B2" s="1" t="s">
@@ -30305,7 +30297,7 @@
       </c>
     </row>
     <row r="4" spans="2:12" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="J4" s="92"/>
+      <c r="J4" s="90"/>
     </row>
     <row r="28" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B28" s="11" t="s">
@@ -30326,7 +30318,7 @@
     </row>
     <row r="31" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B31" s="4" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
     </row>
     <row r="32" spans="2:6" x14ac:dyDescent="0.25">
@@ -30360,25 +30352,25 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.6640625" style="93" customWidth="1"/>
-    <col min="2" max="2" width="19.44140625" style="95" customWidth="1"/>
-    <col min="3" max="3" width="17.44140625" style="95" customWidth="1"/>
-    <col min="4" max="4" width="17.44140625" style="95" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.109375" style="95"/>
+    <col min="1" max="1" width="2.6640625" style="91" customWidth="1"/>
+    <col min="2" max="2" width="19.44140625" style="93" customWidth="1"/>
+    <col min="3" max="3" width="17.44140625" style="93" customWidth="1"/>
+    <col min="4" max="4" width="17.44140625" style="93" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.109375" style="93"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B1" s="117"/>
-      <c r="C1" s="117"/>
-      <c r="D1" s="117"/>
-      <c r="E1" s="117"/>
-      <c r="F1" s="117"/>
-      <c r="G1" s="117"/>
-      <c r="H1" s="117"/>
-      <c r="I1" s="94"/>
-      <c r="J1" s="94"/>
-      <c r="K1" s="94"/>
-      <c r="L1" s="94"/>
+      <c r="B1" s="115"/>
+      <c r="C1" s="115"/>
+      <c r="D1" s="115"/>
+      <c r="E1" s="115"/>
+      <c r="F1" s="115"/>
+      <c r="G1" s="115"/>
+      <c r="H1" s="115"/>
+      <c r="I1" s="92"/>
+      <c r="J1" s="92"/>
+      <c r="K1" s="92"/>
+      <c r="L1" s="92"/>
     </row>
     <row r="2" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B2" s="1" t="s">
@@ -30392,20 +30384,20 @@
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B5" s="96"/>
+      <c r="B5" s="94"/>
       <c r="F5" s="29"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B6" s="96"/>
-      <c r="C6" s="116" t="s">
+      <c r="B6" s="94"/>
+      <c r="C6" s="114" t="s">
         <v>84</v>
       </c>
-      <c r="D6" s="116"/>
+      <c r="D6" s="114"/>
       <c r="E6" s="29"/>
       <c r="G6" s="29"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B7" s="97" t="s">
+      <c r="B7" s="95" t="s">
         <v>83</v>
       </c>
       <c r="C7" s="43" t="s">
@@ -30419,7 +30411,7 @@
       <c r="G7" s="29"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" s="93" t="e">
+      <c r="A8" s="91" t="e">
         <f t="array" aca="1" ref="A8" ca="1">INDEX(fy_range, MATCH(0, COUNTIF($A$7:A7, fy_range), 0))</f>
         <v>#REF!</v>
       </c>
@@ -30436,11 +30428,11 @@
         <v>#REF!</v>
       </c>
       <c r="E8" s="29"/>
-      <c r="F8" s="98"/>
-      <c r="G8" s="98"/>
+      <c r="F8" s="96"/>
+      <c r="G8" s="96"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" s="93" t="e">
+      <c r="A9" s="91" t="e">
         <f t="array" aca="1" ref="A9" ca="1">INDEX(fy_range, MATCH(0, COUNTIF($A$7:A8, fy_range), 0))</f>
         <v>#REF!</v>
       </c>
@@ -30457,12 +30449,12 @@
         <v>#REF!</v>
       </c>
       <c r="E9" s="29"/>
-      <c r="F9" s="98"/>
-      <c r="G9" s="98"/>
-      <c r="I9" s="98"/>
+      <c r="F9" s="96"/>
+      <c r="G9" s="96"/>
+      <c r="I9" s="96"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" s="93" t="e">
+      <c r="A10" s="91" t="e">
         <f t="array" aca="1" ref="A10" ca="1">INDEX(fy_range, MATCH(0, COUNTIF($A$7:A9, fy_range), 0))</f>
         <v>#REF!</v>
       </c>
@@ -30479,12 +30471,12 @@
         <v>#REF!</v>
       </c>
       <c r="E10" s="29"/>
-      <c r="F10" s="98"/>
-      <c r="G10" s="98"/>
-      <c r="I10" s="98"/>
+      <c r="F10" s="96"/>
+      <c r="G10" s="96"/>
+      <c r="I10" s="96"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" s="93" t="e">
+      <c r="A11" s="91" t="e">
         <f t="array" aca="1" ref="A11" ca="1">INDEX(fy_range, MATCH(0, COUNTIF($A$7:A10, fy_range), 0))</f>
         <v>#REF!</v>
       </c>
@@ -30501,12 +30493,12 @@
         <v>#REF!</v>
       </c>
       <c r="E11" s="29"/>
-      <c r="F11" s="98"/>
-      <c r="G11" s="98"/>
-      <c r="I11" s="98"/>
+      <c r="F11" s="96"/>
+      <c r="G11" s="96"/>
+      <c r="I11" s="96"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A12" s="93" t="e">
+      <c r="A12" s="91" t="e">
         <f t="array" aca="1" ref="A12" ca="1">INDEX(fy_range, MATCH(0, COUNTIF($A$7:A11, fy_range), 0))</f>
         <v>#REF!</v>
       </c>
@@ -30523,13 +30515,13 @@
         <v>#REF!</v>
       </c>
       <c r="E12" s="29"/>
-      <c r="F12" s="98"/>
-      <c r="G12" s="98"/>
-      <c r="I12" s="98"/>
-      <c r="J12" s="96"/>
+      <c r="F12" s="96"/>
+      <c r="G12" s="96"/>
+      <c r="I12" s="96"/>
+      <c r="J12" s="94"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A13" s="93" t="e">
+      <c r="A13" s="91" t="e">
         <f t="array" aca="1" ref="A13" ca="1">INDEX(fy_range, MATCH(0, COUNTIF($A$7:A12, fy_range), 0))</f>
         <v>#REF!</v>
       </c>
@@ -30546,13 +30538,13 @@
         <v>#REF!</v>
       </c>
       <c r="E13" s="32"/>
-      <c r="F13" s="98"/>
-      <c r="G13" s="98"/>
-      <c r="I13" s="98"/>
-      <c r="J13" s="96"/>
+      <c r="F13" s="96"/>
+      <c r="G13" s="96"/>
+      <c r="I13" s="96"/>
+      <c r="J13" s="94"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A14" s="93" t="e">
+      <c r="A14" s="91" t="e">
         <f t="array" aca="1" ref="A14" ca="1">INDEX(fy_range, MATCH(0, COUNTIF($A$7:A13, fy_range), 0))</f>
         <v>#REF!</v>
       </c>
@@ -30569,13 +30561,13 @@
         <v>#REF!</v>
       </c>
       <c r="E14" s="32"/>
-      <c r="F14" s="98"/>
-      <c r="G14" s="98"/>
-      <c r="I14" s="98"/>
-      <c r="J14" s="96"/>
+      <c r="F14" s="96"/>
+      <c r="G14" s="96"/>
+      <c r="I14" s="96"/>
+      <c r="J14" s="94"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A15" s="93" t="e">
+      <c r="A15" s="91" t="e">
         <f t="array" aca="1" ref="A15" ca="1">INDEX(fy_range, MATCH(0, COUNTIF($A$7:A14, fy_range), 0))</f>
         <v>#REF!</v>
       </c>
@@ -30592,13 +30584,13 @@
         <v>#REF!</v>
       </c>
       <c r="E15" s="32"/>
-      <c r="F15" s="98"/>
-      <c r="G15" s="98"/>
-      <c r="I15" s="98"/>
-      <c r="J15" s="96"/>
+      <c r="F15" s="96"/>
+      <c r="G15" s="96"/>
+      <c r="I15" s="96"/>
+      <c r="J15" s="94"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A16" s="99" t="e">
+      <c r="A16" s="97" t="e">
         <f t="array" aca="1" ref="A16" ca="1">INDEX(fy_range, MATCH(0, COUNTIF($A$7:A15, fy_range), 0))</f>
         <v>#REF!</v>
       </c>
@@ -30615,11 +30607,11 @@
         <v>#REF!</v>
       </c>
       <c r="E16" s="32"/>
-      <c r="I16" s="98"/>
-      <c r="J16" s="96"/>
+      <c r="I16" s="96"/>
+      <c r="J16" s="94"/>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17" s="99" t="e">
+      <c r="A17" s="97" t="e">
         <f t="array" aca="1" ref="A17" ca="1">INDEX(fy_range, MATCH(0, COUNTIF($A$7:A16, fy_range), 0))</f>
         <v>#REF!</v>
       </c>
@@ -30638,20 +30630,20 @@
       <c r="E17" s="29"/>
       <c r="F17" s="29"/>
       <c r="G17" s="29"/>
-      <c r="H17" s="96"/>
-      <c r="I17" s="96"/>
-      <c r="J17" s="96"/>
+      <c r="H17" s="94"/>
+      <c r="I17" s="94"/>
+      <c r="J17" s="94"/>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B18" s="96"/>
+      <c r="B18" s="94"/>
       <c r="C18" s="29"/>
       <c r="D18" s="29"/>
       <c r="E18" s="29"/>
       <c r="F18" s="29"/>
       <c r="G18" s="29"/>
-      <c r="H18" s="96"/>
-      <c r="I18" s="96"/>
-      <c r="J18" s="96"/>
+      <c r="H18" s="94"/>
+      <c r="I18" s="94"/>
+      <c r="J18" s="94"/>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B19" s="11" t="s">
@@ -30670,7 +30662,7 @@
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B22" s="4" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
@@ -30711,18 +30703,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:13" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B1" s="115"/>
-      <c r="C1" s="115"/>
-      <c r="D1" s="115"/>
-      <c r="E1" s="115"/>
-      <c r="F1" s="115"/>
-      <c r="G1" s="115"/>
-      <c r="H1" s="115"/>
-      <c r="I1" s="115"/>
-      <c r="J1" s="115"/>
-      <c r="K1" s="115"/>
-      <c r="L1" s="115"/>
-      <c r="M1" s="115"/>
+      <c r="B1" s="113"/>
+      <c r="C1" s="113"/>
+      <c r="D1" s="113"/>
+      <c r="E1" s="113"/>
+      <c r="F1" s="113"/>
+      <c r="G1" s="113"/>
+      <c r="H1" s="113"/>
+      <c r="I1" s="113"/>
+      <c r="J1" s="113"/>
+      <c r="K1" s="113"/>
+      <c r="L1" s="113"/>
+      <c r="M1" s="113"/>
     </row>
     <row r="2" spans="2:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B2" s="1" t="s">
@@ -30731,12 +30723,12 @@
     </row>
     <row r="3" spans="2:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B3" s="1" t="e">
-        <f ca="1" xml:space="preserve"> "by Health Board of Residence; " &amp; calculation!K10</f>
+        <f ca="1" xml:space="preserve"> "by NHS Board of Residence; " &amp; calculation!K10</f>
         <v>#REF!</v>
       </c>
     </row>
     <row r="4" spans="2:13" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="J4" s="92" t="e">
+      <c r="J4" s="90" t="e">
         <f ca="1" xml:space="preserve"> "Financial year ending 31st March 20" &amp; RIGHT([0]!fy_max, 2)</f>
         <v>#REF!</v>
       </c>
@@ -30760,7 +30752,7 @@
     </row>
     <row r="37" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B37" s="4" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
     </row>
     <row r="38" spans="2:6" x14ac:dyDescent="0.25">
@@ -30771,12 +30763,12 @@
     </row>
     <row r="39" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B39" s="64" t="s">
-        <v>156</v>
+        <v>164</v>
       </c>
     </row>
     <row r="40" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B40" s="64" t="s">
-        <v>157</v>
+        <v>165</v>
       </c>
     </row>
   </sheetData>
@@ -30810,15 +30802,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B1" s="115"/>
-      <c r="C1" s="115"/>
-      <c r="D1" s="115"/>
-      <c r="E1" s="115"/>
-      <c r="F1" s="115"/>
-      <c r="G1" s="115"/>
-      <c r="H1" s="115"/>
-      <c r="I1" s="115"/>
-      <c r="J1" s="115"/>
+      <c r="B1" s="113"/>
+      <c r="C1" s="113"/>
+      <c r="D1" s="113"/>
+      <c r="E1" s="113"/>
+      <c r="F1" s="113"/>
+      <c r="G1" s="113"/>
+      <c r="H1" s="113"/>
+      <c r="I1" s="113"/>
+      <c r="J1" s="113"/>
       <c r="K1" s="66"/>
     </row>
     <row r="2" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
@@ -30828,7 +30820,7 @@
     </row>
     <row r="3" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B3" s="1" t="e">
-        <f ca="1" xml:space="preserve"> "by Health Board of Residence; " &amp; [0]!fy_max &amp; calculation!$B$4</f>
+        <f ca="1" xml:space="preserve"> "by NHS Board of Residence; " &amp; [0]!fy_max &amp; calculation!$B$4</f>
         <v>#REF!</v>
       </c>
     </row>
@@ -30837,7 +30829,7 @@
     </row>
     <row r="5" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B5" s="75" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C5" s="76" t="e">
         <f ca="1">CONCATENATE([0]!fy_max, calculation!$B$4)</f>
@@ -30852,7 +30844,7 @@
     </row>
     <row r="6" spans="2:11" ht="16.2" x14ac:dyDescent="0.25">
       <c r="B6" s="77" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C6" s="53" t="e">
         <f ca="1">VLOOKUP(CONCATENATE([0]!fy_max, "hb", $B6), [0]!data_range, 5, FALSE)</f>
@@ -30882,7 +30874,7 @@
     </row>
     <row r="8" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B8" s="78" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C8" s="54" t="e">
         <f ca="1">VLOOKUP(CONCATENATE([0]!fy_max, "hb", $B8), [0]!data_range, 5, FALSE)</f>
@@ -30944,7 +30936,7 @@
     </row>
     <row r="12" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B12" s="78" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C12" s="54" t="e">
         <f ca="1">VLOOKUP(CONCATENATE([0]!fy_max, "hb", $B12), [0]!data_range, 5, FALSE)</f>
@@ -31104,7 +31096,7 @@
     </row>
     <row r="24" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B24" s="4" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="J24" s="73"/>
       <c r="K24" s="73"/>
@@ -31119,14 +31111,14 @@
     </row>
     <row r="26" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B26" s="64" t="s">
-        <v>156</v>
+        <v>164</v>
       </c>
       <c r="J26" s="73"/>
       <c r="K26" s="73"/>
     </row>
     <row r="27" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B27" s="64" t="s">
-        <v>157</v>
+        <v>165</v>
       </c>
       <c r="J27" s="73"/>
       <c r="K27" s="73"/>
@@ -31198,18 +31190,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:13" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B1" s="115"/>
-      <c r="C1" s="115"/>
-      <c r="D1" s="115"/>
-      <c r="E1" s="115"/>
-      <c r="F1" s="115"/>
-      <c r="G1" s="115"/>
-      <c r="H1" s="115"/>
-      <c r="I1" s="115"/>
-      <c r="J1" s="115"/>
-      <c r="K1" s="115"/>
-      <c r="L1" s="115"/>
-      <c r="M1" s="115"/>
+      <c r="B1" s="113"/>
+      <c r="C1" s="113"/>
+      <c r="D1" s="113"/>
+      <c r="E1" s="113"/>
+      <c r="F1" s="113"/>
+      <c r="G1" s="113"/>
+      <c r="H1" s="113"/>
+      <c r="I1" s="113"/>
+      <c r="J1" s="113"/>
+      <c r="K1" s="113"/>
+      <c r="L1" s="113"/>
+      <c r="M1" s="113"/>
     </row>
     <row r="2" spans="2:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B2" s="1" t="s">
@@ -31218,12 +31210,12 @@
     </row>
     <row r="3" spans="2:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B3" s="1" t="e">
-        <f ca="1" xml:space="preserve"> "by Age and Gender; " &amp; [0]!fy_max &amp; calculation!$B$4</f>
+        <f ca="1" xml:space="preserve"> "by Age and Sex; " &amp; [0]!fy_max &amp; calculation!$B$4</f>
         <v>#REF!</v>
       </c>
     </row>
     <row r="4" spans="2:13" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="L4" s="100" t="e">
+      <c r="L4" s="98" t="e">
         <f ca="1" xml:space="preserve"> "Financial year ending 31st March 20" &amp; RIGHT([0]!fy_max, 2)</f>
         <v>#REF!</v>
       </c>
@@ -31247,7 +31239,7 @@
     </row>
     <row r="31" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B31" s="4" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
     </row>
     <row r="32" spans="2:6" x14ac:dyDescent="0.25">
@@ -31277,7 +31269,9 @@
   </sheetPr>
   <dimension ref="B1:Q27"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
@@ -31288,15 +31282,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:17" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B1" s="115"/>
-      <c r="C1" s="115"/>
-      <c r="D1" s="115"/>
-      <c r="E1" s="115"/>
-      <c r="F1" s="115"/>
-      <c r="G1" s="115"/>
-      <c r="H1" s="115"/>
-      <c r="I1" s="115"/>
-      <c r="J1" s="115"/>
+      <c r="B1" s="113"/>
+      <c r="C1" s="113"/>
+      <c r="D1" s="113"/>
+      <c r="E1" s="113"/>
+      <c r="F1" s="113"/>
+      <c r="G1" s="113"/>
+      <c r="H1" s="113"/>
+      <c r="I1" s="113"/>
+      <c r="J1" s="113"/>
       <c r="K1" s="66"/>
       <c r="L1" s="66"/>
       <c r="M1" s="66"/>
@@ -31308,7 +31302,7 @@
     </row>
     <row r="3" spans="2:17" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B3" s="1" t="e">
-        <f ca="1" xml:space="preserve"> "by Age and Gender; " &amp; [0]!fy_max &amp; calculation!$B$4</f>
+        <f ca="1" xml:space="preserve"> "by Age and Sex; " &amp; [0]!fy_max &amp; calculation!$B$4</f>
         <v>#REF!</v>
       </c>
     </row>
@@ -31322,39 +31316,39 @@
     </row>
     <row r="6" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B6" s="78"/>
-      <c r="C6" s="118" t="s">
+      <c r="C6" s="116" t="s">
         <v>104</v>
       </c>
-      <c r="D6" s="118"/>
-      <c r="E6" s="118"/>
-      <c r="F6" s="118"/>
-      <c r="G6" s="118"/>
-      <c r="H6" s="118"/>
+      <c r="D6" s="116"/>
+      <c r="E6" s="116"/>
+      <c r="F6" s="116"/>
+      <c r="G6" s="116"/>
+      <c r="H6" s="116"/>
       <c r="J6" s="73"/>
       <c r="K6" s="73"/>
       <c r="Q6" s="69"/>
     </row>
     <row r="7" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B7" s="102" t="s">
+      <c r="B7" s="100" t="s">
+        <v>167</v>
+      </c>
+      <c r="C7" s="101" t="s">
         <v>105</v>
       </c>
-      <c r="C7" s="103" t="s">
+      <c r="D7" s="101" t="s">
         <v>106</v>
       </c>
-      <c r="D7" s="103" t="s">
+      <c r="E7" s="101" t="s">
         <v>107</v>
       </c>
-      <c r="E7" s="103" t="s">
+      <c r="F7" s="101" t="s">
         <v>108</v>
       </c>
-      <c r="F7" s="103" t="s">
+      <c r="G7" s="101" t="s">
         <v>109</v>
       </c>
-      <c r="G7" s="103" t="s">
+      <c r="H7" s="101" t="s">
         <v>110</v>
-      </c>
-      <c r="H7" s="103" t="s">
-        <v>111</v>
       </c>
       <c r="J7" s="73"/>
       <c r="K7" s="73"/>
@@ -31362,7 +31356,7 @@
     </row>
     <row r="8" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B8" s="78" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C8" s="54" t="e">
         <f ca="1">VLOOKUP(CONCATENATE([0]!fy_max, "age/sex", C$7, " ", $B8), [0]!data_range, 5, FALSE)</f>
@@ -31394,7 +31388,7 @@
     </row>
     <row r="9" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B9" s="78" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C9" s="54" t="e">
         <f ca="1">VLOOKUP(CONCATENATE([0]!fy_max, "age/sex", C$7, " ", $B9), [0]!data_range, 5, FALSE)</f>
@@ -31425,8 +31419,8 @@
       <c r="Q9" s="69"/>
     </row>
     <row r="10" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B10" s="104" t="s">
-        <v>113</v>
+      <c r="B10" s="102" t="s">
+        <v>112</v>
       </c>
       <c r="C10" s="55" t="e">
         <f ca="1">VLOOKUP(CONCATENATE([0]!fy_max, "age/sex", C$7, " ", $B10), [0]!data_range, 5, FALSE)</f>
@@ -31472,7 +31466,7 @@
       <c r="Q12" s="69"/>
     </row>
     <row r="13" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B13" s="101"/>
+      <c r="B13" s="99"/>
       <c r="J13" s="73"/>
       <c r="K13" s="73"/>
       <c r="Q13" s="69"/>
@@ -31487,7 +31481,7 @@
     </row>
     <row r="15" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B15" s="4" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="J15" s="73"/>
       <c r="K15" s="73"/>
@@ -31589,22 +31583,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:13" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B1" s="115"/>
-      <c r="C1" s="115"/>
-      <c r="D1" s="115"/>
-      <c r="E1" s="115"/>
-      <c r="F1" s="115"/>
-      <c r="G1" s="115"/>
-      <c r="H1" s="115"/>
-      <c r="I1" s="115"/>
-      <c r="J1" s="115"/>
-      <c r="K1" s="115"/>
-      <c r="L1" s="115"/>
-      <c r="M1" s="115"/>
+      <c r="B1" s="113"/>
+      <c r="C1" s="113"/>
+      <c r="D1" s="113"/>
+      <c r="E1" s="113"/>
+      <c r="F1" s="113"/>
+      <c r="G1" s="113"/>
+      <c r="H1" s="113"/>
+      <c r="I1" s="113"/>
+      <c r="J1" s="113"/>
+      <c r="K1" s="113"/>
+      <c r="L1" s="113"/>
+      <c r="M1" s="113"/>
     </row>
     <row r="2" spans="2:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B2" s="1" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
     </row>
     <row r="3" spans="2:13" ht="15.6" x14ac:dyDescent="0.3">
@@ -31614,7 +31608,7 @@
       </c>
     </row>
     <row r="4" spans="2:13" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="J4" s="92" t="e">
+      <c r="J4" s="90" t="e">
         <f ca="1" xml:space="preserve"> "Financial year ending 31st March 20" &amp; RIGHT([0]!fy_max, 2)</f>
         <v>#REF!</v>
       </c>
@@ -31646,7 +31640,7 @@
     </row>
     <row r="32" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B32" s="4" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="C32" s="74"/>
       <c r="D32" s="74"/>
@@ -31660,31 +31654,31 @@
       </c>
     </row>
     <row r="34" spans="2:13" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="119" t="s">
-        <v>169</v>
-      </c>
-      <c r="C34" s="119"/>
-      <c r="D34" s="119"/>
-      <c r="E34" s="119"/>
-      <c r="F34" s="119"/>
-      <c r="G34" s="119"/>
-      <c r="H34" s="119"/>
-      <c r="I34" s="119"/>
-      <c r="J34" s="119"/>
-      <c r="K34" s="119"/>
-      <c r="L34" s="119"/>
-      <c r="M34" s="119"/>
+      <c r="B34" s="117" t="s">
+        <v>168</v>
+      </c>
+      <c r="C34" s="117"/>
+      <c r="D34" s="117"/>
+      <c r="E34" s="117"/>
+      <c r="F34" s="117"/>
+      <c r="G34" s="117"/>
+      <c r="H34" s="117"/>
+      <c r="I34" s="117"/>
+      <c r="J34" s="117"/>
+      <c r="K34" s="117"/>
+      <c r="L34" s="117"/>
+      <c r="M34" s="117"/>
     </row>
     <row r="35" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B35" s="58" t="s">
+        <v>113</v>
+      </c>
+      <c r="G35" s="33" t="s">
         <v>114</v>
       </c>
-      <c r="G35" s="33" t="s">
-        <v>115</v>
-      </c>
     </row>
     <row r="36" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B36" s="101"/>
+      <c r="B36" s="99"/>
     </row>
     <row r="37" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B37" s="3"/>
@@ -31742,21 +31736,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:20" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B1" s="115"/>
-      <c r="C1" s="115"/>
-      <c r="D1" s="115"/>
-      <c r="E1" s="115"/>
-      <c r="F1" s="115"/>
-      <c r="G1" s="115"/>
-      <c r="H1" s="115"/>
-      <c r="I1" s="115"/>
-      <c r="J1" s="115"/>
-      <c r="K1" s="115"/>
-      <c r="L1" s="115"/>
-      <c r="M1" s="115"/>
-      <c r="N1" s="115"/>
-      <c r="O1" s="115"/>
-      <c r="P1" s="115"/>
+      <c r="B1" s="113"/>
+      <c r="C1" s="113"/>
+      <c r="D1" s="113"/>
+      <c r="E1" s="113"/>
+      <c r="F1" s="113"/>
+      <c r="G1" s="113"/>
+      <c r="H1" s="113"/>
+      <c r="I1" s="113"/>
+      <c r="J1" s="113"/>
+      <c r="K1" s="113"/>
+      <c r="L1" s="113"/>
+      <c r="M1" s="113"/>
+      <c r="N1" s="113"/>
+      <c r="O1" s="113"/>
+      <c r="P1" s="113"/>
       <c r="Q1" s="66"/>
       <c r="R1" s="66"/>
       <c r="S1" s="66"/>
@@ -31764,7 +31758,7 @@
     </row>
     <row r="2" spans="2:20" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B2" s="1" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
@@ -31788,110 +31782,110 @@
       <c r="I3" s="1"/>
     </row>
     <row r="5" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="D5" s="105"/>
-      <c r="E5" s="105"/>
-      <c r="F5" s="105"/>
-      <c r="G5" s="105"/>
-      <c r="H5" s="105"/>
-      <c r="I5" s="105"/>
+      <c r="D5" s="103"/>
+      <c r="E5" s="103"/>
+      <c r="F5" s="103"/>
+      <c r="G5" s="103"/>
+      <c r="H5" s="103"/>
+      <c r="I5" s="103"/>
     </row>
     <row r="6" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B6" s="50" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C6" s="51" t="e">
         <f ca="1">CONCATENATE([0]!fy_max, calculation!$B$4)</f>
         <v>#REF!</v>
       </c>
-      <c r="D6" s="105"/>
-      <c r="E6" s="105"/>
-      <c r="F6" s="105"/>
-      <c r="G6" s="105"/>
-      <c r="H6" s="105"/>
-      <c r="I6" s="105"/>
+      <c r="D6" s="103"/>
+      <c r="E6" s="103"/>
+      <c r="F6" s="103"/>
+      <c r="G6" s="103"/>
+      <c r="H6" s="103"/>
+      <c r="I6" s="103"/>
     </row>
     <row r="7" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B7" s="106" t="s">
-        <v>125</v>
+      <c r="B7" s="104" t="s">
+        <v>124</v>
       </c>
       <c r="C7" s="54" t="e">
         <f ca="1">VLOOKUP(CONCATENATE([0]!fy_max, "simd quintile", $B7), [0]!data_range, 5, FALSE)</f>
         <v>#REF!</v>
       </c>
-      <c r="D7" s="105"/>
-      <c r="E7" s="105"/>
-      <c r="F7" s="105"/>
-      <c r="G7" s="105"/>
-      <c r="H7" s="105"/>
-      <c r="I7" s="105"/>
+      <c r="D7" s="103"/>
+      <c r="E7" s="103"/>
+      <c r="F7" s="103"/>
+      <c r="G7" s="103"/>
+      <c r="H7" s="103"/>
+      <c r="I7" s="103"/>
     </row>
     <row r="8" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B8" s="106">
+      <c r="B8" s="104">
         <v>2</v>
       </c>
       <c r="C8" s="54" t="e">
         <f ca="1">VLOOKUP(CONCATENATE([0]!fy_max, "simd quintile", $B8), [0]!data_range, 5, FALSE)</f>
         <v>#REF!</v>
       </c>
-      <c r="D8" s="105"/>
-      <c r="E8" s="105"/>
-      <c r="F8" s="105"/>
-      <c r="G8" s="105"/>
-      <c r="H8" s="105"/>
-      <c r="I8" s="105"/>
+      <c r="D8" s="103"/>
+      <c r="E8" s="103"/>
+      <c r="F8" s="103"/>
+      <c r="G8" s="103"/>
+      <c r="H8" s="103"/>
+      <c r="I8" s="103"/>
     </row>
     <row r="9" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B9" s="106">
+      <c r="B9" s="104">
         <v>3</v>
       </c>
       <c r="C9" s="54" t="e">
         <f ca="1">VLOOKUP(CONCATENATE([0]!fy_max, "simd quintile", $B9), [0]!data_range, 5, FALSE)</f>
         <v>#REF!</v>
       </c>
-      <c r="D9" s="105"/>
-      <c r="E9" s="105"/>
-      <c r="F9" s="105"/>
-      <c r="G9" s="105"/>
-      <c r="H9" s="105"/>
-      <c r="I9" s="105"/>
+      <c r="D9" s="103"/>
+      <c r="E9" s="103"/>
+      <c r="F9" s="103"/>
+      <c r="G9" s="103"/>
+      <c r="H9" s="103"/>
+      <c r="I9" s="103"/>
     </row>
     <row r="10" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B10" s="106">
+      <c r="B10" s="104">
         <v>4</v>
       </c>
       <c r="C10" s="54" t="e">
         <f ca="1">VLOOKUP(CONCATENATE([0]!fy_max, "simd quintile", $B10), [0]!data_range, 5, FALSE)</f>
         <v>#REF!</v>
       </c>
-      <c r="D10" s="105"/>
-      <c r="E10" s="105"/>
-      <c r="F10" s="105"/>
-      <c r="G10" s="105"/>
-      <c r="H10" s="105"/>
-      <c r="I10" s="105"/>
+      <c r="D10" s="103"/>
+      <c r="E10" s="103"/>
+      <c r="F10" s="103"/>
+      <c r="G10" s="103"/>
+      <c r="H10" s="103"/>
+      <c r="I10" s="103"/>
     </row>
     <row r="11" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B11" s="107" t="s">
-        <v>126</v>
+      <c r="B11" s="105" t="s">
+        <v>125</v>
       </c>
       <c r="C11" s="55" t="e">
         <f ca="1">VLOOKUP(CONCATENATE([0]!fy_max, "simd quintile", $B11), [0]!data_range, 5, FALSE)</f>
         <v>#REF!</v>
       </c>
-      <c r="D11" s="105"/>
-      <c r="E11" s="105"/>
-      <c r="F11" s="105"/>
-      <c r="G11" s="105"/>
-      <c r="H11" s="105"/>
-      <c r="I11" s="105"/>
+      <c r="D11" s="103"/>
+      <c r="E11" s="103"/>
+      <c r="F11" s="103"/>
+      <c r="G11" s="103"/>
+      <c r="H11" s="103"/>
+      <c r="I11" s="103"/>
     </row>
     <row r="12" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="D12" s="105"/>
-      <c r="E12" s="105"/>
-      <c r="F12" s="105"/>
-      <c r="G12" s="105"/>
-      <c r="H12" s="105"/>
-      <c r="I12" s="105"/>
+      <c r="D12" s="103"/>
+      <c r="E12" s="103"/>
+      <c r="F12" s="103"/>
+      <c r="G12" s="103"/>
+      <c r="H12" s="103"/>
+      <c r="I12" s="103"/>
     </row>
     <row r="13" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B13" s="11" t="s">
@@ -31929,7 +31923,7 @@
     </row>
     <row r="16" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B16" s="4" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="C16" s="74"/>
       <c r="D16" s="74"/>
@@ -31943,27 +31937,27 @@
       </c>
     </row>
     <row r="18" spans="2:13" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="119" t="s">
-        <v>169</v>
-      </c>
-      <c r="C18" s="119"/>
-      <c r="D18" s="119"/>
-      <c r="E18" s="119"/>
-      <c r="F18" s="119"/>
-      <c r="G18" s="119"/>
-      <c r="H18" s="119"/>
-      <c r="I18" s="119"/>
-      <c r="J18" s="119"/>
-      <c r="K18" s="119"/>
-      <c r="L18" s="119"/>
-      <c r="M18" s="119"/>
+      <c r="B18" s="117" t="s">
+        <v>168</v>
+      </c>
+      <c r="C18" s="117"/>
+      <c r="D18" s="117"/>
+      <c r="E18" s="117"/>
+      <c r="F18" s="117"/>
+      <c r="G18" s="117"/>
+      <c r="H18" s="117"/>
+      <c r="I18" s="117"/>
+      <c r="J18" s="117"/>
+      <c r="K18" s="117"/>
+      <c r="L18" s="117"/>
+      <c r="M18" s="117"/>
     </row>
     <row r="19" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B19" s="58" t="s">
+        <v>113</v>
+      </c>
+      <c r="E19" s="33" t="s">
         <v>114</v>
-      </c>
-      <c r="E19" s="33" t="s">
-        <v>115</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Final changes to markdown files and templates to reflect most recent publication.
</commit_message>
<xml_diff>
--- a/reference-files/figures-template.xlsx
+++ b/reference-files/figures-template.xlsx
@@ -39,12 +39,12 @@
     <definedName name="_xlnm.Print_Area" localSheetId="13">'External Causes of Deaths'!$A$2:$E$49</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">'Figure 1'!$B$1:$L$32</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="2">OFFSET('Figure 1 Background Data'!$B$1:$H$1, 0, 0, calculation!$B$7+14, 9)</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="3">'Figure 2'!$B$1:$M$40</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="4">'Figure 2 Background Data'!$B$1:$J$27</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="3">'Figure 2'!$B$1:$M$41</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="4">'Figure 2 Background Data'!$B$1:$J$28</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="5">'Figure 3'!$B$1:$M$32</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="6">'Figure 3 Background Data'!$B$1:$J$16</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="7">'Figure 4'!$B$2:$N$35</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="8">'Figure 4 Background Data'!$B$2:$J$19</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="7">'Figure 4'!$B$2:$N$36</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="8">'Figure 4 Background Data'!$B$2:$J$20</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="9">'Figure 5'!$B$2:$O$35</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="10">'Figure 5 Background Data'!$B$2:$J$17</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="11">'Figure A3.1'!$B$1:$L$30</definedName>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="173">
   <si>
     <t>External causes of death excluded from analysis</t>
   </si>
@@ -406,9 +406,6 @@
     <t>Deprivation Category</t>
   </si>
   <si>
-    <t>http://www.gov.scot/Topics/Statistics/About/Methodology/UrbanRuralClassification</t>
-  </si>
-  <si>
     <t>Urban Rural 6-fold Classification</t>
   </si>
   <si>
@@ -487,9 +484,6 @@
     <t>NHS Greater Glasgow and Clyde</t>
   </si>
   <si>
-    <t xml:space="preserve">2. For more information on Urban / Rural classification see </t>
-  </si>
-  <si>
     <t>Old Measure</t>
   </si>
   <si>
@@ -550,19 +544,10 @@
     <t>NHS Board relates to location of residence at time of death and is based on the 2019 boundaries.</t>
   </si>
   <si>
-    <t>2. The NHS Board of Residence is the usual place of residence prior to death.</t>
-  </si>
-  <si>
-    <t>3. NHS Boards are based on the NHS Board boundaries which came into effect 1st April 2014.</t>
-  </si>
-  <si>
     <t>NHS Board of Residence</t>
   </si>
   <si>
     <t>Sex</t>
-  </si>
-  <si>
-    <t>2. Data are analysed by the 2020 ‘Scotland level’ Scottish Index of Multiple Deprivation (SIMD) population weighted quintiles. Each quintile consists of approximately 20% of the population living in Scotland, with deprivation quintile 1 indicating the population living in the most deprived areas.</t>
   </si>
   <si>
     <t>ᴾ</t>
@@ -573,6 +558,24 @@
   <si>
     <t xml:space="preserve">Hospital activity data is estimated to be 96% complete at Scotland level. However this is much lower for Forth Valley (50%) and as a result estimated figures for 2019/20 have been calculated for NHS Forth Valley and the Health and Social Care Partnerships within this area. These estimates have also been included in the Scotland figure. </t>
   </si>
+  <si>
+    <t>COVID-19 footnote</t>
+  </si>
+  <si>
+    <t>3. The NHS Board of Residence is the usual place of residence prior to death.</t>
+  </si>
+  <si>
+    <t>4. NHS Boards are based on the NHS Board boundaries which came into effect 1st April 2014.</t>
+  </si>
+  <si>
+    <t>3. Data are analysed by the 2020 ‘Scotland level’ Scottish Index of Multiple Deprivation (SIMD) population weighted quintiles. Each quintile consists of approximately 20% of the population living in Scotland, with deprivation quintile 1 indicating the population living in the most deprived areas.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3. For more information on Urban / Rural classification see </t>
+  </si>
+  <si>
+    <t>https://www.gov.scot/publications/scottish-government-urban-rural-classification-2016/pages/1/</t>
+  </si>
 </sst>
 </file>
 
@@ -581,7 +584,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="28" x14ac:knownFonts="1">
+  <fonts count="30" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -757,6 +760,21 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="8"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -836,7 +854,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="14">
+  <cellStyleXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
@@ -857,8 +875,9 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="123">
+  <cellXfs count="128">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
@@ -1050,6 +1069,9 @@
     <xf numFmtId="0" fontId="20" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -1077,13 +1099,16 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="7" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="14" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="14" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="14">
+  <cellStyles count="15">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Hyperlink 2" xfId="8"/>
+    <cellStyle name="Hyperlink 3" xfId="14"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="2"/>
     <cellStyle name="Normal 2 2" xfId="6"/>
@@ -1390,6 +1415,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -1438,6 +1464,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0" sourceLinked="0"/>
@@ -1453,6 +1480,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1692,6 +1720,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -1730,6 +1759,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0" sourceLinked="0"/>
@@ -1745,6 +1775,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1877,6 +1908,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -1915,6 +1947,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0" sourceLinked="0"/>
@@ -2110,6 +2143,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0" sourceLinked="0"/>
@@ -2439,6 +2473,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2540,6 +2575,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2620,6 +2656,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4339,7 +4376,7 @@
     <row r="7" spans="1:28" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="21"/>
       <c r="B7" s="11" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C7" s="11"/>
       <c r="D7" s="11"/>
@@ -4371,7 +4408,7 @@
     <row r="8" spans="1:28" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="21"/>
       <c r="B8" s="11" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C8" s="11"/>
       <c r="D8" s="11"/>
@@ -4403,7 +4440,7 @@
     <row r="9" spans="1:28" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="21"/>
       <c r="B9" s="11" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C9" s="11"/>
       <c r="D9" s="11"/>
@@ -4435,7 +4472,7 @@
     <row r="10" spans="1:28" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="21"/>
       <c r="B10" s="11" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C10" s="11"/>
       <c r="D10" s="11"/>
@@ -4467,7 +4504,7 @@
     <row r="11" spans="1:28" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="21"/>
       <c r="B11" s="11" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C11" s="11"/>
       <c r="D11" s="11"/>
@@ -4561,7 +4598,7 @@
     <row r="14" spans="1:28" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="21"/>
       <c r="B14" s="24" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C14" s="21"/>
       <c r="D14" s="21"/>
@@ -4720,22 +4757,22 @@
     <row r="19" spans="1:28" s="24" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A19" s="21"/>
       <c r="B19" s="82"/>
-      <c r="C19" s="122" t="s">
-        <v>170</v>
-      </c>
-      <c r="D19" s="122"/>
-      <c r="E19" s="122"/>
-      <c r="F19" s="122"/>
-      <c r="G19" s="122"/>
-      <c r="H19" s="122"/>
-      <c r="I19" s="122"/>
-      <c r="J19" s="122"/>
-      <c r="K19" s="122"/>
-      <c r="L19" s="122"/>
-      <c r="M19" s="122"/>
-      <c r="N19" s="122"/>
-      <c r="O19" s="122"/>
-      <c r="P19" s="122"/>
+      <c r="C19" s="113" t="s">
+        <v>165</v>
+      </c>
+      <c r="D19" s="113"/>
+      <c r="E19" s="113"/>
+      <c r="F19" s="113"/>
+      <c r="G19" s="113"/>
+      <c r="H19" s="113"/>
+      <c r="I19" s="113"/>
+      <c r="J19" s="113"/>
+      <c r="K19" s="113"/>
+      <c r="L19" s="113"/>
+      <c r="M19" s="113"/>
+      <c r="N19" s="113"/>
+      <c r="O19" s="113"/>
+      <c r="P19" s="113"/>
       <c r="Q19" s="21"/>
       <c r="R19" s="21"/>
       <c r="S19" s="21"/>
@@ -5189,7 +5226,7 @@
     <row r="45" spans="2:16" s="21" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="B45" s="86"/>
       <c r="C45" s="87" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D45" s="74"/>
       <c r="E45" s="74"/>
@@ -5223,7 +5260,7 @@
         <v>78</v>
       </c>
       <c r="C48" s="21" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="49" spans="1:16" s="21" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
@@ -5313,7 +5350,7 @@
   <sheetPr codeName="Sheet10">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:M36"/>
+  <dimension ref="B1:M37"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
@@ -5328,21 +5365,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:13" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B1" s="113"/>
-      <c r="C1" s="113"/>
-      <c r="D1" s="113"/>
-      <c r="E1" s="113"/>
-      <c r="F1" s="113"/>
-      <c r="G1" s="113"/>
-      <c r="H1" s="113"/>
-      <c r="I1" s="113"/>
-      <c r="J1" s="113"/>
-      <c r="K1" s="113"/>
-      <c r="L1" s="113"/>
+      <c r="B1" s="114"/>
+      <c r="C1" s="114"/>
+      <c r="D1" s="114"/>
+      <c r="E1" s="114"/>
+      <c r="F1" s="114"/>
+      <c r="G1" s="114"/>
+      <c r="H1" s="114"/>
+      <c r="I1" s="114"/>
+      <c r="J1" s="114"/>
+      <c r="K1" s="114"/>
+      <c r="L1" s="114"/>
     </row>
     <row r="2" spans="2:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B2" s="1" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="3" spans="2:13" ht="15.6" x14ac:dyDescent="0.3">
@@ -5376,7 +5413,7 @@
     </row>
     <row r="34" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B34" s="4" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="35" spans="2:7" x14ac:dyDescent="0.25">
@@ -5386,11 +5423,17 @@
       </c>
     </row>
     <row r="36" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B36" s="58" t="s">
-        <v>143</v>
-      </c>
-      <c r="G36" s="33" t="s">
-        <v>116</v>
+      <c r="B36" s="64" t="str">
+        <f>"2. " &amp; calculation!B19</f>
+        <v>2. The increase in 2020/21 is likely due to the impact of COVID-19 on hospital stays. Please see Notes tab for more information.</v>
+      </c>
+    </row>
+    <row r="37" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B37" s="58" t="s">
+        <v>171</v>
+      </c>
+      <c r="G37" s="124" t="s">
+        <v>172</v>
       </c>
     </row>
   </sheetData>
@@ -5399,8 +5442,8 @@
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B31" location="'External Causes of Deaths'!A1" display="External causes of death excluded from analysis"/>
-    <hyperlink ref="G36" r:id="rId1"/>
     <hyperlink ref="B31:F31" location="'External Causes of Deaths'!A1" display="External causes of death excluded from analysis"/>
+    <hyperlink ref="G37" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="90" orientation="landscape" r:id="rId2"/>
@@ -5413,7 +5456,7 @@
   <sheetPr codeName="Sheet11">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:S19"/>
+  <dimension ref="B1:S20"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
@@ -5432,19 +5475,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:19" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B1" s="113"/>
-      <c r="C1" s="113"/>
-      <c r="D1" s="113"/>
-      <c r="E1" s="113"/>
-      <c r="F1" s="113"/>
-      <c r="G1" s="113"/>
-      <c r="H1" s="113"/>
-      <c r="I1" s="113"/>
-      <c r="J1" s="113"/>
-      <c r="K1" s="113"/>
-      <c r="L1" s="113"/>
-      <c r="M1" s="113"/>
-      <c r="N1" s="113"/>
+      <c r="B1" s="114"/>
+      <c r="C1" s="114"/>
+      <c r="D1" s="114"/>
+      <c r="E1" s="114"/>
+      <c r="F1" s="114"/>
+      <c r="G1" s="114"/>
+      <c r="H1" s="114"/>
+      <c r="I1" s="114"/>
+      <c r="J1" s="114"/>
+      <c r="K1" s="114"/>
+      <c r="L1" s="114"/>
+      <c r="M1" s="114"/>
+      <c r="N1" s="114"/>
       <c r="O1" s="66"/>
       <c r="P1" s="66"/>
       <c r="Q1" s="66"/>
@@ -5453,7 +5496,7 @@
     </row>
     <row r="2" spans="2:19" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B2" s="1" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
@@ -5478,7 +5521,7 @@
     </row>
     <row r="6" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B6" s="52" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C6" s="43" t="e">
         <f ca="1">CONCATENATE([0]!fy_max, calculation!$B$4)</f>
@@ -5487,7 +5530,7 @@
     </row>
     <row r="7" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B7" s="45" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C7" s="53" t="e">
         <f ca="1">VLOOKUP(CONCATENATE([0]!fy_max, "urban rural 6", $B7), [0]!data_range, 5, FALSE)</f>
@@ -5496,7 +5539,7 @@
     </row>
     <row r="8" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B8" s="47" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C8" s="54" t="e">
         <f ca="1">VLOOKUP(CONCATENATE([0]!fy_max, "urban rural 6", $B8), [0]!data_range, 5, FALSE)</f>
@@ -5505,7 +5548,7 @@
     </row>
     <row r="9" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B9" s="47" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C9" s="54" t="e">
         <f ca="1">VLOOKUP(CONCATENATE([0]!fy_max, "urban rural 6", $B9), [0]!data_range, 5, FALSE)</f>
@@ -5514,7 +5557,7 @@
     </row>
     <row r="10" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B10" s="47" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C10" s="54" t="e">
         <f ca="1">VLOOKUP(CONCATENATE([0]!fy_max, "urban rural 6", $B10), [0]!data_range, 5, FALSE)</f>
@@ -5523,7 +5566,7 @@
     </row>
     <row r="11" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B11" s="47" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C11" s="54" t="e">
         <f ca="1">VLOOKUP(CONCATENATE([0]!fy_max, "urban rural 6", $B11), [0]!data_range, 5, FALSE)</f>
@@ -5532,7 +5575,7 @@
     </row>
     <row r="12" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B12" s="49" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C12" s="55" t="e">
         <f ca="1">VLOOKUP(CONCATENATE([0]!fy_max, "urban rural 6", $B12), [0]!data_range, 5, FALSE)</f>
@@ -5576,7 +5619,7 @@
     </row>
     <row r="17" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B17" s="4" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C17" s="4"/>
       <c r="D17" s="4"/>
@@ -5592,12 +5635,18 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B19" s="58" t="s">
-        <v>143</v>
-      </c>
-      <c r="D19" s="33" t="s">
-        <v>116</v>
+    <row r="19" spans="2:9" s="126" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="64" t="str">
+        <f>"2. " &amp; calculation!B19</f>
+        <v>2. The increase in 2020/21 is likely due to the impact of COVID-19 on hospital stays. Please see Notes tab for more information.</v>
+      </c>
+    </row>
+    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B20" s="58" t="s">
+        <v>171</v>
+      </c>
+      <c r="D20" s="127" t="s">
+        <v>172</v>
       </c>
     </row>
   </sheetData>
@@ -5607,7 +5656,7 @@
   <hyperlinks>
     <hyperlink ref="B14" location="'External Causes of Deaths'!A1" display="External causes of death excluded from analysis"/>
     <hyperlink ref="B14:J14" location="'External Causes of Deaths'!A1" display="External causes of death excluded from analysis"/>
-    <hyperlink ref="D19" r:id="rId1"/>
+    <hyperlink ref="D20" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="92" orientation="landscape" r:id="rId2"/>
@@ -5619,7 +5668,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:L30"/>
+  <dimension ref="B1:L31"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
@@ -5632,21 +5681,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B1" s="113"/>
-      <c r="C1" s="113"/>
-      <c r="D1" s="113"/>
-      <c r="E1" s="113"/>
-      <c r="F1" s="113"/>
-      <c r="G1" s="113"/>
-      <c r="H1" s="113"/>
-      <c r="I1" s="113"/>
-      <c r="J1" s="113"/>
-      <c r="K1" s="113"/>
-      <c r="L1" s="113"/>
+      <c r="B1" s="114"/>
+      <c r="C1" s="114"/>
+      <c r="D1" s="114"/>
+      <c r="E1" s="114"/>
+      <c r="F1" s="114"/>
+      <c r="G1" s="114"/>
+      <c r="H1" s="114"/>
+      <c r="I1" s="114"/>
+      <c r="J1" s="114"/>
+      <c r="K1" s="114"/>
+      <c r="L1" s="114"/>
     </row>
     <row r="2" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B2" s="1" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="3" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
@@ -5677,13 +5726,19 @@
     </row>
     <row r="29" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B29" s="4" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="30" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B30" s="64" t="e">
         <f ca="1" xml:space="preserve"> "1. " &amp; calculation!$B$14</f>
         <v>#REF!</v>
+      </c>
+    </row>
+    <row r="31" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B31" s="125" t="str">
+        <f>"2. " &amp; calculation!B19</f>
+        <v>2. The increase in 2020/21 is likely due to the impact of COVID-19 on hospital stays. Please see Notes tab for more information.</v>
       </c>
     </row>
   </sheetData>
@@ -5705,7 +5760,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:L22"/>
+  <dimension ref="A1:L23"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
@@ -5719,13 +5774,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B1" s="115"/>
-      <c r="C1" s="115"/>
-      <c r="D1" s="115"/>
-      <c r="E1" s="115"/>
-      <c r="F1" s="115"/>
-      <c r="G1" s="115"/>
-      <c r="H1" s="115"/>
+      <c r="B1" s="116"/>
+      <c r="C1" s="116"/>
+      <c r="D1" s="116"/>
+      <c r="E1" s="116"/>
+      <c r="F1" s="116"/>
+      <c r="G1" s="116"/>
+      <c r="H1" s="116"/>
       <c r="I1" s="92"/>
       <c r="J1" s="92"/>
       <c r="K1" s="92"/>
@@ -5733,7 +5788,7 @@
     </row>
     <row r="2" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B2" s="1" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
@@ -5751,10 +5806,10 @@
         <v>83</v>
       </c>
       <c r="C6" s="43" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="D6" s="59" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="E6" s="29"/>
       <c r="F6" s="29"/>
@@ -6012,13 +6067,19 @@
     </row>
     <row r="21" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B21" s="4" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="22" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B22" s="64" t="e">
         <f ca="1" xml:space="preserve"> "1. " &amp; calculation!$B$14</f>
         <v>#REF!</v>
+      </c>
+    </row>
+    <row r="23" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B23" s="4" t="str">
+        <f>"2. " &amp; calculation!B19</f>
+        <v>2. The increase in 2020/21 is likely due to the impact of COVID-19 on hospital stays. Please see Notes tab for more information.</v>
       </c>
     </row>
   </sheetData>
@@ -6650,10 +6711,10 @@
     </row>
     <row r="20" spans="1:4" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="30"/>
-      <c r="B20" s="118" t="s">
+      <c r="B20" s="119" t="s">
         <v>28</v>
       </c>
-      <c r="C20" s="118"/>
+      <c r="C20" s="119"/>
       <c r="D20" s="13"/>
     </row>
     <row r="21" spans="1:4" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -6818,16 +6879,16 @@
     </row>
     <row r="37" spans="1:4" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="30"/>
-      <c r="B37" s="119"/>
-      <c r="C37" s="119"/>
+      <c r="B37" s="120"/>
+      <c r="C37" s="120"/>
       <c r="D37" s="13"/>
     </row>
     <row r="38" spans="1:4" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="30"/>
-      <c r="B38" s="118" t="s">
+      <c r="B38" s="119" t="s">
         <v>61</v>
       </c>
-      <c r="C38" s="118"/>
+      <c r="C38" s="119"/>
       <c r="D38" s="13"/>
     </row>
     <row r="39" spans="1:4" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -6895,7 +6956,7 @@
     <row r="47" spans="1:4" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="30"/>
       <c r="B47" s="5" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C47" s="2"/>
       <c r="D47" s="13"/>
@@ -7847,22 +7908,22 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="34" t="s">
+        <v>117</v>
+      </c>
+      <c r="B1" s="34" t="s">
         <v>118</v>
       </c>
-      <c r="B1" s="34" t="s">
+      <c r="C1" s="34" t="s">
         <v>119</v>
       </c>
-      <c r="C1" s="34" t="s">
+      <c r="D1" s="34" t="s">
         <v>120</v>
       </c>
-      <c r="D1" s="34" t="s">
+      <c r="E1" s="34" t="s">
         <v>121</v>
       </c>
-      <c r="E1" s="34" t="s">
+      <c r="F1" s="34" t="s">
         <v>122</v>
-      </c>
-      <c r="F1" s="34" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -29869,7 +29930,9 @@
   <sheetPr codeName="Sheet14"/>
   <dimension ref="A1:K24"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
@@ -30005,7 +30068,7 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="38" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B1" s="39">
         <f>COUNTA(data!B:B)-1</f>
@@ -30014,7 +30077,7 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="38" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B2" s="39">
         <f>COUNTA(data!1:1)</f>
@@ -30023,33 +30086,33 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="38" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B4" s="56" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="38" t="s">
+        <v>135</v>
+      </c>
+      <c r="B5" s="39" t="s">
         <v>136</v>
-      </c>
-      <c r="B5" s="39" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="38" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B6" s="108" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="I6" s="38"/>
       <c r="K6" s="38"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="38" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B7" s="39">
         <v>10</v>
@@ -30160,15 +30223,15 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="38" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B13" s="38" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="38" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B14" s="39" t="e">
         <f ca="1">"Data for "&amp; $K$9 &amp;" are provisional. Please see Notes tab for more information."</f>
@@ -30177,34 +30240,34 @@
     </row>
     <row r="15" spans="1:11" ht="80.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="61" t="s">
-        <v>151</v>
-      </c>
-      <c r="B15" s="120" t="e">
+        <v>149</v>
+      </c>
+      <c r="B15" s="121" t="e">
         <f ca="1">IF($B$13 = "provisional", "Hospital data and ", "") &amp; "National Records of Scotland deaths data " &amp; IF($B$13 = "provisional", "are", "is") &amp; " provisional for " &amp; $K$9 &amp;". " &amp; IF($B$13 = "provisional", "This publication will be updated in October 20" &amp; RIGHT($K$9,2) &amp; ". " &amp; $B$16, "")</f>
         <v>#REF!</v>
       </c>
-      <c r="C15" s="120"/>
-      <c r="D15" s="120"/>
-      <c r="E15" s="120"/>
-      <c r="F15" s="120"/>
-      <c r="G15" s="120"/>
-      <c r="H15" s="120"/>
-      <c r="I15" s="120"/>
+      <c r="C15" s="121"/>
+      <c r="D15" s="121"/>
+      <c r="E15" s="121"/>
+      <c r="F15" s="121"/>
+      <c r="G15" s="121"/>
+      <c r="H15" s="121"/>
+      <c r="I15" s="121"/>
     </row>
     <row r="16" spans="1:11" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="38" t="s">
-        <v>152</v>
-      </c>
-      <c r="B16" s="121" t="s">
-        <v>171</v>
-      </c>
-      <c r="C16" s="120"/>
-      <c r="D16" s="120"/>
-      <c r="E16" s="120"/>
-      <c r="F16" s="120"/>
-      <c r="G16" s="120"/>
-      <c r="H16" s="120"/>
-      <c r="I16" s="120"/>
+        <v>150</v>
+      </c>
+      <c r="B16" s="122" t="s">
+        <v>166</v>
+      </c>
+      <c r="C16" s="121"/>
+      <c r="D16" s="121"/>
+      <c r="E16" s="121"/>
+      <c r="F16" s="121"/>
+      <c r="G16" s="121"/>
+      <c r="H16" s="121"/>
+      <c r="I16" s="121"/>
     </row>
     <row r="17" spans="1:9" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="38"/>
@@ -30228,7 +30291,13 @@
       <c r="H18" s="63"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" s="38"/>
+      <c r="A19" s="38" t="s">
+        <v>167</v>
+      </c>
+      <c r="B19" s="39" t="str">
+        <f>"The increase in 2020/21 is likely due to the impact of COVID-19 on hospital stays. Please see Notes tab for more information."</f>
+        <v>The increase in 2020/21 is likely due to the impact of COVID-19 on hospital stays. Please see Notes tab for more information.</v>
+      </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="38"/>
@@ -30260,7 +30329,7 @@
   <sheetPr codeName="Sheet2">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:L32"/>
+  <dimension ref="B1:L33"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
@@ -30273,17 +30342,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B1" s="113"/>
-      <c r="C1" s="113"/>
-      <c r="D1" s="113"/>
-      <c r="E1" s="113"/>
-      <c r="F1" s="113"/>
-      <c r="G1" s="113"/>
-      <c r="H1" s="113"/>
-      <c r="I1" s="113"/>
-      <c r="J1" s="113"/>
-      <c r="K1" s="113"/>
-      <c r="L1" s="113"/>
+      <c r="B1" s="114"/>
+      <c r="C1" s="114"/>
+      <c r="D1" s="114"/>
+      <c r="E1" s="114"/>
+      <c r="F1" s="114"/>
+      <c r="G1" s="114"/>
+      <c r="H1" s="114"/>
+      <c r="I1" s="114"/>
+      <c r="J1" s="114"/>
+      <c r="K1" s="114"/>
+      <c r="L1" s="114"/>
     </row>
     <row r="2" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B2" s="1" t="s">
@@ -30318,13 +30387,19 @@
     </row>
     <row r="31" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B31" s="4" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="32" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B32" s="64" t="e">
         <f ca="1" xml:space="preserve"> "1. " &amp; calculation!B14</f>
         <v>#REF!</v>
+      </c>
+    </row>
+    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B33" s="123" t="str">
+        <f>"2. " &amp; calculation!B19</f>
+        <v>2. The increase in 2020/21 is likely due to the impact of COVID-19 on hospital stays. Please see Notes tab for more information.</v>
       </c>
     </row>
   </sheetData>
@@ -30346,7 +30421,7 @@
   <sheetPr codeName="Sheet3">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:L23"/>
+  <dimension ref="A1:L24"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
@@ -30360,13 +30435,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B1" s="115"/>
-      <c r="C1" s="115"/>
-      <c r="D1" s="115"/>
-      <c r="E1" s="115"/>
-      <c r="F1" s="115"/>
-      <c r="G1" s="115"/>
-      <c r="H1" s="115"/>
+      <c r="B1" s="116"/>
+      <c r="C1" s="116"/>
+      <c r="D1" s="116"/>
+      <c r="E1" s="116"/>
+      <c r="F1" s="116"/>
+      <c r="G1" s="116"/>
+      <c r="H1" s="116"/>
       <c r="I1" s="92"/>
       <c r="J1" s="92"/>
       <c r="K1" s="92"/>
@@ -30389,10 +30464,10 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B6" s="94"/>
-      <c r="C6" s="114" t="s">
+      <c r="C6" s="115" t="s">
         <v>84</v>
       </c>
-      <c r="D6" s="114"/>
+      <c r="D6" s="115"/>
       <c r="E6" s="29"/>
       <c r="G6" s="29"/>
     </row>
@@ -30662,13 +30737,19 @@
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B22" s="4" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B23" s="4" t="e">
         <f ca="1" xml:space="preserve"> "1. " &amp; calculation!$B$14</f>
         <v>#REF!</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B24" s="123" t="str">
+        <f>"2. " &amp; calculation!B19</f>
+        <v>2. The increase in 2020/21 is likely due to the impact of COVID-19 on hospital stays. Please see Notes tab for more information.</v>
       </c>
     </row>
   </sheetData>
@@ -30690,7 +30771,7 @@
   <sheetPr codeName="Sheet4">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:M40"/>
+  <dimension ref="B1:M41"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
@@ -30703,18 +30784,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:13" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B1" s="113"/>
-      <c r="C1" s="113"/>
-      <c r="D1" s="113"/>
-      <c r="E1" s="113"/>
-      <c r="F1" s="113"/>
-      <c r="G1" s="113"/>
-      <c r="H1" s="113"/>
-      <c r="I1" s="113"/>
-      <c r="J1" s="113"/>
-      <c r="K1" s="113"/>
-      <c r="L1" s="113"/>
-      <c r="M1" s="113"/>
+      <c r="B1" s="114"/>
+      <c r="C1" s="114"/>
+      <c r="D1" s="114"/>
+      <c r="E1" s="114"/>
+      <c r="F1" s="114"/>
+      <c r="G1" s="114"/>
+      <c r="H1" s="114"/>
+      <c r="I1" s="114"/>
+      <c r="J1" s="114"/>
+      <c r="K1" s="114"/>
+      <c r="L1" s="114"/>
+      <c r="M1" s="114"/>
     </row>
     <row r="2" spans="2:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B2" s="1" t="s">
@@ -30752,7 +30833,7 @@
     </row>
     <row r="37" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B37" s="4" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="38" spans="2:6" x14ac:dyDescent="0.25">
@@ -30762,13 +30843,19 @@
       </c>
     </row>
     <row r="39" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B39" s="64" t="s">
-        <v>164</v>
+      <c r="B39" s="64" t="str">
+        <f>"2. " &amp; calculation!B19</f>
+        <v>2. The increase in 2020/21 is likely due to the impact of COVID-19 on hospital stays. Please see Notes tab for more information.</v>
       </c>
     </row>
     <row r="40" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B40" s="64" t="s">
-        <v>165</v>
+        <v>168</v>
+      </c>
+    </row>
+    <row r="41" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B41" s="64" t="s">
+        <v>169</v>
       </c>
     </row>
   </sheetData>
@@ -30789,7 +30876,7 @@
   <sheetPr codeName="Sheet5">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:K36"/>
+  <dimension ref="B1:K37"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
@@ -30802,15 +30889,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B1" s="113"/>
-      <c r="C1" s="113"/>
-      <c r="D1" s="113"/>
-      <c r="E1" s="113"/>
-      <c r="F1" s="113"/>
-      <c r="G1" s="113"/>
-      <c r="H1" s="113"/>
-      <c r="I1" s="113"/>
-      <c r="J1" s="113"/>
+      <c r="B1" s="114"/>
+      <c r="C1" s="114"/>
+      <c r="D1" s="114"/>
+      <c r="E1" s="114"/>
+      <c r="F1" s="114"/>
+      <c r="G1" s="114"/>
+      <c r="H1" s="114"/>
+      <c r="I1" s="114"/>
+      <c r="J1" s="114"/>
       <c r="K1" s="66"/>
     </row>
     <row r="2" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
@@ -30829,7 +30916,7 @@
     </row>
     <row r="5" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B5" s="75" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="C5" s="76" t="e">
         <f ca="1">CONCATENATE([0]!fy_max, calculation!$B$4)</f>
@@ -30844,7 +30931,7 @@
     </row>
     <row r="6" spans="2:11" ht="16.2" x14ac:dyDescent="0.25">
       <c r="B6" s="77" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C6" s="53" t="e">
         <f ca="1">VLOOKUP(CONCATENATE([0]!fy_max, "hb", $B6), [0]!data_range, 5, FALSE)</f>
@@ -30874,7 +30961,7 @@
     </row>
     <row r="8" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B8" s="78" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C8" s="54" t="e">
         <f ca="1">VLOOKUP(CONCATENATE([0]!fy_max, "hb", $B8), [0]!data_range, 5, FALSE)</f>
@@ -30936,7 +31023,7 @@
     </row>
     <row r="12" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B12" s="78" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C12" s="54" t="e">
         <f ca="1">VLOOKUP(CONCATENATE([0]!fy_max, "hb", $B12), [0]!data_range, 5, FALSE)</f>
@@ -31096,7 +31183,7 @@
     </row>
     <row r="24" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B24" s="4" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="J24" s="73"/>
       <c r="K24" s="73"/>
@@ -31110,20 +31197,24 @@
       <c r="K25" s="73"/>
     </row>
     <row r="26" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B26" s="64" t="s">
-        <v>164</v>
+      <c r="B26" s="64" t="str">
+        <f>"2. " &amp; calculation!B19</f>
+        <v>2. The increase in 2020/21 is likely due to the impact of COVID-19 on hospital stays. Please see Notes tab for more information.</v>
       </c>
       <c r="J26" s="73"/>
       <c r="K26" s="73"/>
     </row>
     <row r="27" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B27" s="64" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="J27" s="73"/>
       <c r="K27" s="73"/>
     </row>
     <row r="28" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B28" s="64" t="s">
+        <v>169</v>
+      </c>
       <c r="J28" s="73"/>
       <c r="K28" s="73"/>
     </row>
@@ -31158,6 +31249,10 @@
     <row r="36" spans="10:11" x14ac:dyDescent="0.25">
       <c r="J36" s="73"/>
       <c r="K36" s="73"/>
+    </row>
+    <row r="37" spans="10:11" x14ac:dyDescent="0.25">
+      <c r="J37" s="73"/>
+      <c r="K37" s="73"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -31177,7 +31272,7 @@
   <sheetPr codeName="Sheet6">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:M32"/>
+  <dimension ref="B1:M33"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
@@ -31190,18 +31285,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:13" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B1" s="113"/>
-      <c r="C1" s="113"/>
-      <c r="D1" s="113"/>
-      <c r="E1" s="113"/>
-      <c r="F1" s="113"/>
-      <c r="G1" s="113"/>
-      <c r="H1" s="113"/>
-      <c r="I1" s="113"/>
-      <c r="J1" s="113"/>
-      <c r="K1" s="113"/>
-      <c r="L1" s="113"/>
-      <c r="M1" s="113"/>
+      <c r="B1" s="114"/>
+      <c r="C1" s="114"/>
+      <c r="D1" s="114"/>
+      <c r="E1" s="114"/>
+      <c r="F1" s="114"/>
+      <c r="G1" s="114"/>
+      <c r="H1" s="114"/>
+      <c r="I1" s="114"/>
+      <c r="J1" s="114"/>
+      <c r="K1" s="114"/>
+      <c r="L1" s="114"/>
+      <c r="M1" s="114"/>
     </row>
     <row r="2" spans="2:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B2" s="1" t="s">
@@ -31239,13 +31334,19 @@
     </row>
     <row r="31" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B31" s="4" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="32" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B32" s="64" t="e">
         <f ca="1" xml:space="preserve"> "1. " &amp; calculation!$B$14</f>
         <v>#REF!</v>
+      </c>
+    </row>
+    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B33" s="123" t="str">
+        <f>"2. " &amp; calculation!B19</f>
+        <v>2. The increase in 2020/21 is likely due to the impact of COVID-19 on hospital stays. Please see Notes tab for more information.</v>
       </c>
     </row>
   </sheetData>
@@ -31269,9 +31370,7 @@
   </sheetPr>
   <dimension ref="B1:Q27"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
-    </sheetView>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
@@ -31282,15 +31381,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:17" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B1" s="113"/>
-      <c r="C1" s="113"/>
-      <c r="D1" s="113"/>
-      <c r="E1" s="113"/>
-      <c r="F1" s="113"/>
-      <c r="G1" s="113"/>
-      <c r="H1" s="113"/>
-      <c r="I1" s="113"/>
-      <c r="J1" s="113"/>
+      <c r="B1" s="114"/>
+      <c r="C1" s="114"/>
+      <c r="D1" s="114"/>
+      <c r="E1" s="114"/>
+      <c r="F1" s="114"/>
+      <c r="G1" s="114"/>
+      <c r="H1" s="114"/>
+      <c r="I1" s="114"/>
+      <c r="J1" s="114"/>
       <c r="K1" s="66"/>
       <c r="L1" s="66"/>
       <c r="M1" s="66"/>
@@ -31316,21 +31415,21 @@
     </row>
     <row r="6" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B6" s="78"/>
-      <c r="C6" s="116" t="s">
+      <c r="C6" s="117" t="s">
         <v>104</v>
       </c>
-      <c r="D6" s="116"/>
-      <c r="E6" s="116"/>
-      <c r="F6" s="116"/>
-      <c r="G6" s="116"/>
-      <c r="H6" s="116"/>
+      <c r="D6" s="117"/>
+      <c r="E6" s="117"/>
+      <c r="F6" s="117"/>
+      <c r="G6" s="117"/>
+      <c r="H6" s="117"/>
       <c r="J6" s="73"/>
       <c r="K6" s="73"/>
       <c r="Q6" s="69"/>
     </row>
     <row r="7" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B7" s="100" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="C7" s="101" t="s">
         <v>105</v>
@@ -31356,7 +31455,7 @@
     </row>
     <row r="8" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B8" s="78" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C8" s="54" t="e">
         <f ca="1">VLOOKUP(CONCATENATE([0]!fy_max, "age/sex", C$7, " ", $B8), [0]!data_range, 5, FALSE)</f>
@@ -31481,7 +31580,7 @@
     </row>
     <row r="15" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B15" s="4" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="J15" s="73"/>
       <c r="K15" s="73"/>
@@ -31496,57 +31595,61 @@
       <c r="K16" s="73"/>
       <c r="Q16" s="69"/>
     </row>
-    <row r="17" spans="10:17" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B17" s="123" t="str">
+        <f>"2. " &amp; calculation!B19</f>
+        <v>2. The increase in 2020/21 is likely due to the impact of COVID-19 on hospital stays. Please see Notes tab for more information.</v>
+      </c>
       <c r="J17" s="73"/>
       <c r="K17" s="73"/>
       <c r="Q17" s="69"/>
     </row>
-    <row r="18" spans="10:17" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:17" x14ac:dyDescent="0.25">
       <c r="J18" s="73"/>
       <c r="K18" s="73"/>
       <c r="Q18" s="69"/>
     </row>
-    <row r="19" spans="10:17" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:17" x14ac:dyDescent="0.25">
       <c r="J19" s="73"/>
       <c r="K19" s="73"/>
       <c r="Q19" s="69"/>
     </row>
-    <row r="20" spans="10:17" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:17" x14ac:dyDescent="0.25">
       <c r="J20" s="73"/>
       <c r="K20" s="73"/>
       <c r="Q20" s="69"/>
     </row>
-    <row r="21" spans="10:17" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:17" x14ac:dyDescent="0.25">
       <c r="J21" s="73"/>
       <c r="K21" s="73"/>
       <c r="Q21" s="69"/>
     </row>
-    <row r="22" spans="10:17" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:17" x14ac:dyDescent="0.25">
       <c r="J22" s="73"/>
       <c r="K22" s="73"/>
       <c r="Q22" s="69"/>
     </row>
-    <row r="23" spans="10:17" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:17" x14ac:dyDescent="0.25">
       <c r="J23" s="73"/>
       <c r="K23" s="73"/>
       <c r="L23" s="73"/>
     </row>
-    <row r="24" spans="10:17" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:17" x14ac:dyDescent="0.25">
       <c r="J24" s="73"/>
       <c r="K24" s="73"/>
       <c r="L24" s="73"/>
     </row>
-    <row r="25" spans="10:17" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:17" x14ac:dyDescent="0.25">
       <c r="J25" s="73"/>
       <c r="K25" s="73"/>
       <c r="L25" s="73"/>
     </row>
-    <row r="26" spans="10:17" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:17" x14ac:dyDescent="0.25">
       <c r="J26" s="73"/>
       <c r="K26" s="73"/>
       <c r="L26" s="73"/>
     </row>
-    <row r="27" spans="10:17" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:17" x14ac:dyDescent="0.25">
       <c r="J27" s="73"/>
       <c r="K27" s="73"/>
       <c r="L27" s="73"/>
@@ -31570,7 +31673,7 @@
   <sheetPr codeName="Sheet8">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:M41"/>
+  <dimension ref="B1:M42"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
@@ -31583,22 +31686,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:13" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B1" s="113"/>
-      <c r="C1" s="113"/>
-      <c r="D1" s="113"/>
-      <c r="E1" s="113"/>
-      <c r="F1" s="113"/>
-      <c r="G1" s="113"/>
-      <c r="H1" s="113"/>
-      <c r="I1" s="113"/>
-      <c r="J1" s="113"/>
-      <c r="K1" s="113"/>
-      <c r="L1" s="113"/>
-      <c r="M1" s="113"/>
+      <c r="B1" s="114"/>
+      <c r="C1" s="114"/>
+      <c r="D1" s="114"/>
+      <c r="E1" s="114"/>
+      <c r="F1" s="114"/>
+      <c r="G1" s="114"/>
+      <c r="H1" s="114"/>
+      <c r="I1" s="114"/>
+      <c r="J1" s="114"/>
+      <c r="K1" s="114"/>
+      <c r="L1" s="114"/>
+      <c r="M1" s="114"/>
     </row>
     <row r="2" spans="2:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B2" s="1" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="3" spans="2:13" ht="15.6" x14ac:dyDescent="0.3">
@@ -31640,7 +31743,7 @@
     </row>
     <row r="32" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B32" s="4" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C32" s="74"/>
       <c r="D32" s="74"/>
@@ -31653,56 +31756,62 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="34" spans="2:13" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="117" t="s">
-        <v>168</v>
-      </c>
-      <c r="C34" s="117"/>
-      <c r="D34" s="117"/>
-      <c r="E34" s="117"/>
-      <c r="F34" s="117"/>
-      <c r="G34" s="117"/>
-      <c r="H34" s="117"/>
-      <c r="I34" s="117"/>
-      <c r="J34" s="117"/>
-      <c r="K34" s="117"/>
-      <c r="L34" s="117"/>
-      <c r="M34" s="117"/>
-    </row>
-    <row r="35" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B35" s="58" t="s">
+    <row r="34" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B34" s="64" t="str">
+        <f>"2. " &amp; calculation!B19</f>
+        <v>2. The increase in 2020/21 is likely due to the impact of COVID-19 on hospital stays. Please see Notes tab for more information.</v>
+      </c>
+    </row>
+    <row r="35" spans="2:13" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B35" s="118" t="s">
+        <v>170</v>
+      </c>
+      <c r="C35" s="118"/>
+      <c r="D35" s="118"/>
+      <c r="E35" s="118"/>
+      <c r="F35" s="118"/>
+      <c r="G35" s="118"/>
+      <c r="H35" s="118"/>
+      <c r="I35" s="118"/>
+      <c r="J35" s="118"/>
+      <c r="K35" s="118"/>
+      <c r="L35" s="118"/>
+      <c r="M35" s="118"/>
+    </row>
+    <row r="36" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B36" s="58" t="s">
         <v>113</v>
       </c>
-      <c r="G35" s="33" t="s">
+      <c r="G36" s="33" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="36" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B36" s="99"/>
-    </row>
     <row r="37" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B37" s="3"/>
+      <c r="B37" s="99"/>
     </row>
     <row r="38" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B38" s="4"/>
+      <c r="B38" s="3"/>
     </row>
     <row r="39" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B39" s="3"/>
+      <c r="B39" s="4"/>
     </row>
     <row r="40" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B40" s="3"/>
     </row>
     <row r="41" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B41" s="3"/>
+    </row>
+    <row r="42" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B42" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="B1:M1"/>
-    <mergeCell ref="B34:M34"/>
+    <mergeCell ref="B35:M35"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B29" location="'External Causes of Deaths'!A1" display="External causes of death excluded from analysis"/>
-    <hyperlink ref="G35" r:id="rId1"/>
+    <hyperlink ref="G36" r:id="rId1"/>
     <hyperlink ref="B29:F29" location="'External Causes of Deaths'!A1" display="External causes of death excluded from analysis"/>
   </hyperlinks>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
@@ -31716,7 +31825,7 @@
   <sheetPr codeName="Sheet9">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:T19"/>
+  <dimension ref="B1:T20"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
@@ -31736,21 +31845,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:20" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B1" s="113"/>
-      <c r="C1" s="113"/>
-      <c r="D1" s="113"/>
-      <c r="E1" s="113"/>
-      <c r="F1" s="113"/>
-      <c r="G1" s="113"/>
-      <c r="H1" s="113"/>
-      <c r="I1" s="113"/>
-      <c r="J1" s="113"/>
-      <c r="K1" s="113"/>
-      <c r="L1" s="113"/>
-      <c r="M1" s="113"/>
-      <c r="N1" s="113"/>
-      <c r="O1" s="113"/>
-      <c r="P1" s="113"/>
+      <c r="B1" s="114"/>
+      <c r="C1" s="114"/>
+      <c r="D1" s="114"/>
+      <c r="E1" s="114"/>
+      <c r="F1" s="114"/>
+      <c r="G1" s="114"/>
+      <c r="H1" s="114"/>
+      <c r="I1" s="114"/>
+      <c r="J1" s="114"/>
+      <c r="K1" s="114"/>
+      <c r="L1" s="114"/>
+      <c r="M1" s="114"/>
+      <c r="N1" s="114"/>
+      <c r="O1" s="114"/>
+      <c r="P1" s="114"/>
       <c r="Q1" s="66"/>
       <c r="R1" s="66"/>
       <c r="S1" s="66"/>
@@ -31758,7 +31867,7 @@
     </row>
     <row r="2" spans="2:20" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B2" s="1" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
@@ -31806,7 +31915,7 @@
     </row>
     <row r="7" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B7" s="104" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C7" s="54" t="e">
         <f ca="1">VLOOKUP(CONCATENATE([0]!fy_max, "simd quintile", $B7), [0]!data_range, 5, FALSE)</f>
@@ -31866,7 +31975,7 @@
     </row>
     <row r="11" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B11" s="105" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C11" s="55" t="e">
         <f ca="1">VLOOKUP(CONCATENATE([0]!fy_max, "simd quintile", $B11), [0]!data_range, 5, FALSE)</f>
@@ -31923,7 +32032,7 @@
     </row>
     <row r="16" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B16" s="4" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C16" s="74"/>
       <c r="D16" s="74"/>
@@ -31936,39 +32045,45 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="18" spans="2:13" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="117" t="s">
-        <v>168</v>
-      </c>
-      <c r="C18" s="117"/>
-      <c r="D18" s="117"/>
-      <c r="E18" s="117"/>
-      <c r="F18" s="117"/>
-      <c r="G18" s="117"/>
-      <c r="H18" s="117"/>
-      <c r="I18" s="117"/>
-      <c r="J18" s="117"/>
-      <c r="K18" s="117"/>
-      <c r="L18" s="117"/>
-      <c r="M18" s="117"/>
-    </row>
-    <row r="19" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B19" s="58" t="s">
+    <row r="18" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B18" s="64" t="str">
+        <f>"2. " &amp; calculation!B19</f>
+        <v>2. The increase in 2020/21 is likely due to the impact of COVID-19 on hospital stays. Please see Notes tab for more information.</v>
+      </c>
+    </row>
+    <row r="19" spans="2:13" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="118" t="s">
+        <v>170</v>
+      </c>
+      <c r="C19" s="118"/>
+      <c r="D19" s="118"/>
+      <c r="E19" s="118"/>
+      <c r="F19" s="118"/>
+      <c r="G19" s="118"/>
+      <c r="H19" s="118"/>
+      <c r="I19" s="118"/>
+      <c r="J19" s="118"/>
+      <c r="K19" s="118"/>
+      <c r="L19" s="118"/>
+      <c r="M19" s="118"/>
+    </row>
+    <row r="20" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B20" s="58" t="s">
         <v>113</v>
       </c>
-      <c r="E19" s="33" t="s">
+      <c r="E20" s="33" t="s">
         <v>114</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="B1:P1"/>
-    <mergeCell ref="B18:M18"/>
+    <mergeCell ref="B19:M19"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B13" location="'External Causes of Deaths'!A1" display="External causes of death excluded from analysis"/>
     <hyperlink ref="B13:L13" location="'External Causes of Deaths'!A1" display="External causes of death excluded from analysis"/>
-    <hyperlink ref="E19" r:id="rId1"/>
+    <hyperlink ref="E20" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId2"/>

</xml_diff>

<commit_message>
Changes to summary, addition of new main points to report and footnote updated in excel templates
</commit_message>
<xml_diff>
--- a/reference-files/figures-template.xlsx
+++ b/reference-files/figures-template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Y:\18-End-of-Life\Publication\Gaby\reference-files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D3542DC-EE25-4744-9852-8B415B5DCC75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9FBCD0A-FBB6-4ADA-ADE4-EA402E2F30E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="649" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="649" firstSheet="8" activeTab="15" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Notes" sheetId="9" r:id="rId1"/>
@@ -4071,7 +4071,7 @@
   </sheetPr>
   <dimension ref="A1:AB74"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -5495,7 +5495,7 @@
     <row r="36" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B36" s="64" t="str">
         <f>"2. " &amp; calculation!B19</f>
-        <v>2. Figures in 2020/21 and 2021/22 are likely to have been affected by the impact of COVID-19 on hospital stays</v>
+        <v>2. Figures in 2020/21 and 2021/22 are likely to have been affected by the impact of COVID-19 on hospital stays.</v>
       </c>
     </row>
     <row r="37" spans="2:7" x14ac:dyDescent="0.2">
@@ -5708,7 +5708,7 @@
     <row r="19" spans="2:9" s="112" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B19" s="64" t="str">
         <f>"2. " &amp; calculation!B19</f>
-        <v>2. Figures in 2020/21 and 2021/22 are likely to have been affected by the impact of COVID-19 on hospital stays</v>
+        <v>2. Figures in 2020/21 and 2021/22 are likely to have been affected by the impact of COVID-19 on hospital stays.</v>
       </c>
     </row>
     <row r="20" spans="2:9" x14ac:dyDescent="0.2">
@@ -5808,7 +5808,7 @@
     <row r="31" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B31" s="111" t="str">
         <f>"2. " &amp; calculation!B19</f>
-        <v>2. Figures in 2020/21 and 2021/22 are likely to have been affected by the impact of COVID-19 on hospital stays</v>
+        <v>2. Figures in 2020/21 and 2021/22 are likely to have been affected by the impact of COVID-19 on hospital stays.</v>
       </c>
     </row>
   </sheetData>
@@ -6149,7 +6149,7 @@
     <row r="23" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B23" s="4" t="str">
         <f>"2. " &amp; calculation!B19</f>
-        <v>2. Figures in 2020/21 and 2021/22 are likely to have been affected by the impact of COVID-19 on hospital stays</v>
+        <v>2. Figures in 2020/21 and 2021/22 are likely to have been affected by the impact of COVID-19 on hospital stays.</v>
       </c>
     </row>
   </sheetData>
@@ -30000,8 +30000,8 @@
   <sheetPr codeName="Sheet14"/>
   <dimension ref="A1:K24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L25" sqref="L25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -30365,8 +30365,8 @@
         <v>167</v>
       </c>
       <c r="B19" s="39" t="str">
-        <f>"Figures in 2020/21 and 2021/22 are likely to have been affected by the impact of COVID-19 on hospital stays"</f>
-        <v>Figures in 2020/21 and 2021/22 are likely to have been affected by the impact of COVID-19 on hospital stays</v>
+        <f>"Figures in 2020/21 and 2021/22 are likely to have been affected by the impact of COVID-19 on hospital stays."</f>
+        <v>Figures in 2020/21 and 2021/22 are likely to have been affected by the impact of COVID-19 on hospital stays.</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
@@ -30469,7 +30469,7 @@
     <row r="33" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B33" s="109" t="str">
         <f>"2. " &amp; calculation!B19</f>
-        <v>2. Figures in 2020/21 and 2021/22 are likely to have been affected by the impact of COVID-19 on hospital stays</v>
+        <v>2. Figures in 2020/21 and 2021/22 are likely to have been affected by the impact of COVID-19 on hospital stays.</v>
       </c>
     </row>
   </sheetData>
@@ -30819,7 +30819,7 @@
     <row r="24" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B24" s="109" t="str">
         <f>"2. " &amp; calculation!B19</f>
-        <v>2. Figures in 2020/21 and 2021/22 are likely to have been affected by the impact of COVID-19 on hospital stays</v>
+        <v>2. Figures in 2020/21 and 2021/22 are likely to have been affected by the impact of COVID-19 on hospital stays.</v>
       </c>
     </row>
   </sheetData>
@@ -30915,7 +30915,7 @@
     <row r="39" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B39" s="64" t="str">
         <f>"2. " &amp; calculation!B19</f>
-        <v>2. Figures in 2020/21 and 2021/22 are likely to have been affected by the impact of COVID-19 on hospital stays</v>
+        <v>2. Figures in 2020/21 and 2021/22 are likely to have been affected by the impact of COVID-19 on hospital stays.</v>
       </c>
     </row>
     <row r="40" spans="2:6" x14ac:dyDescent="0.2">
@@ -31269,7 +31269,7 @@
     <row r="26" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B26" s="64" t="str">
         <f>"2. " &amp; calculation!B19</f>
-        <v>2. Figures in 2020/21 and 2021/22 are likely to have been affected by the impact of COVID-19 on hospital stays</v>
+        <v>2. Figures in 2020/21 and 2021/22 are likely to have been affected by the impact of COVID-19 on hospital stays.</v>
       </c>
       <c r="J26" s="73"/>
       <c r="K26" s="73"/>
@@ -31416,7 +31416,7 @@
     <row r="33" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B33" s="109" t="str">
         <f>"2. " &amp; calculation!B19</f>
-        <v>2. Figures in 2020/21 and 2021/22 are likely to have been affected by the impact of COVID-19 on hospital stays</v>
+        <v>2. Figures in 2020/21 and 2021/22 are likely to have been affected by the impact of COVID-19 on hospital stays.</v>
       </c>
     </row>
   </sheetData>
@@ -31668,7 +31668,7 @@
     <row r="17" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B17" s="109" t="str">
         <f>"2. " &amp; calculation!B19</f>
-        <v>2. Figures in 2020/21 and 2021/22 are likely to have been affected by the impact of COVID-19 on hospital stays</v>
+        <v>2. Figures in 2020/21 and 2021/22 are likely to have been affected by the impact of COVID-19 on hospital stays.</v>
       </c>
       <c r="J17" s="73"/>
       <c r="K17" s="73"/>
@@ -31829,7 +31829,7 @@
     <row r="34" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B34" s="64" t="str">
         <f>"2. " &amp; calculation!B19</f>
-        <v>2. Figures in 2020/21 and 2021/22 are likely to have been affected by the impact of COVID-19 on hospital stays</v>
+        <v>2. Figures in 2020/21 and 2021/22 are likely to have been affected by the impact of COVID-19 on hospital stays.</v>
       </c>
     </row>
     <row r="35" spans="2:13" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -32118,7 +32118,7 @@
     <row r="18" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B18" s="64" t="str">
         <f>"2. " &amp; calculation!B19</f>
-        <v>2. Figures in 2020/21 and 2021/22 are likely to have been affected by the impact of COVID-19 on hospital stays</v>
+        <v>2. Figures in 2020/21 and 2021/22 are likely to have been affected by the impact of COVID-19 on hospital stays.</v>
       </c>
     </row>
     <row r="19" spans="2:13" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
New templates replaced in March 24
</commit_message>
<xml_diff>
--- a/reference-files/figures-template.xlsx
+++ b/reference-files/figures-template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\stats\irf\18-End-of-Life\Publication\Sissi\end-of-life-pub\reference-files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69D3C0A4-5491-46FA-86AA-BCB2C77389FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{575888F2-14CC-4DF3-9CD4-B64FD278F1FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="649" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="649" firstSheet="4" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Notes" sheetId="9" r:id="rId1"/>
@@ -68,7 +68,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="178">
   <si>
     <t>External causes of death excluded from analysis</t>
   </si>
@@ -373,9 +373,6 @@
     <t>Age Group</t>
   </si>
   <si>
-    <t>0-54</t>
-  </si>
-  <si>
     <t>55-64</t>
   </si>
   <si>
@@ -596,6 +593,15 @@
   </si>
   <si>
     <t>https://www.gov.scot/publications/scottish-government-urban-rural-classification-2020/pages/0/</t>
+  </si>
+  <si>
+    <t>45-54</t>
+  </si>
+  <si>
+    <t>18-44</t>
+  </si>
+  <si>
+    <t>0-17</t>
   </si>
 </sst>
 </file>
@@ -904,7 +910,7 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="113">
+  <cellXfs count="115">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
@@ -1106,9 +1112,6 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" indent="1"/>
     </xf>
@@ -1123,6 +1126,11 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="7" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="15">
@@ -1564,25 +1572,31 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Figure 3 Background Data'!$C$7:$H$7</c:f>
+              <c:f>'Figure 3 Background Data'!$C$7:$J$7</c:f>
               <c:strCache>
-                <c:ptCount val="6"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>0-54</c:v>
+                  <c:v>0-17</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>18-44</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>45-54</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>55-64</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="4">
                   <c:v>65-74</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="5">
                   <c:v>75-84</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="6">
                   <c:v>85+</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="7">
                   <c:v>All Ages</c:v>
                 </c:pt>
               </c:strCache>
@@ -1590,10 +1604,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Figure 3 Background Data'!$C$8:$H$8</c:f>
+              <c:f>'Figure 3 Background Data'!$C$8:$J$8</c:f>
               <c:numCache>
                 <c:formatCode>0.0</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -1610,6 +1624,12 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -1646,25 +1666,31 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Figure 3 Background Data'!$C$7:$H$7</c:f>
+              <c:f>'Figure 3 Background Data'!$C$7:$J$7</c:f>
               <c:strCache>
-                <c:ptCount val="6"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>0-54</c:v>
+                  <c:v>0-17</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>18-44</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>45-54</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>55-64</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="4">
                   <c:v>65-74</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="5">
                   <c:v>75-84</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="6">
                   <c:v>85+</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="7">
                   <c:v>All Ages</c:v>
                 </c:pt>
               </c:strCache>
@@ -1672,10 +1698,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Figure 3 Background Data'!$C$9:$H$9</c:f>
+              <c:f>'Figure 3 Background Data'!$C$9:$J$9</c:f>
               <c:numCache>
                 <c:formatCode>0.0</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -1692,6 +1718,12 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -4089,7 +4121,7 @@
   </sheetPr>
   <dimension ref="A1:AB78"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
@@ -4464,7 +4496,7 @@
     <row r="7" spans="1:28" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="16"/>
       <c r="B7" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
@@ -4496,7 +4528,7 @@
     <row r="8" spans="1:28" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="16"/>
       <c r="B8" s="2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
@@ -4528,7 +4560,7 @@
     <row r="9" spans="1:28" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="16"/>
       <c r="B9" s="2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
@@ -4560,7 +4592,7 @@
     <row r="10" spans="1:28" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="16"/>
       <c r="B10" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
@@ -4592,7 +4624,7 @@
     <row r="11" spans="1:28" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="16"/>
       <c r="B11" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
@@ -4654,7 +4686,7 @@
     <row r="13" spans="1:28" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="16"/>
       <c r="B13" s="16" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C13" s="16"/>
       <c r="D13" s="16"/>
@@ -4686,7 +4718,7 @@
     <row r="14" spans="1:28" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="16"/>
       <c r="B14" s="19" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C14" s="16"/>
       <c r="D14" s="16"/>
@@ -4846,7 +4878,7 @@
       <c r="A19" s="16"/>
       <c r="B19" s="66"/>
       <c r="C19" s="102" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D19" s="102"/>
       <c r="E19" s="102"/>
@@ -4910,7 +4942,7 @@
         <v>74</v>
       </c>
       <c r="C21" s="103" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D21" s="103"/>
       <c r="E21" s="103"/>
@@ -4973,7 +5005,7 @@
         <v>85</v>
       </c>
       <c r="C23" s="97" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D23" s="97"/>
       <c r="E23" s="97"/>
@@ -5412,7 +5444,7 @@
     <row r="49" spans="1:16" s="16" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="B49" s="70"/>
       <c r="C49" s="71" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D49" s="5"/>
       <c r="E49" s="5"/>
@@ -5426,7 +5458,7 @@
     <row r="50" spans="1:16" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B50" s="26"/>
       <c r="C50" s="21" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D50" s="22"/>
       <c r="E50" s="23"/>
@@ -5446,7 +5478,7 @@
         <v>86</v>
       </c>
       <c r="C52" s="16" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="53" spans="1:16" s="16" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
@@ -5456,10 +5488,10 @@
     <row r="54" spans="1:16" s="16" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="67"/>
       <c r="B54" s="94" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C54" s="98" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D54" s="98"/>
       <c r="E54" s="98"/>
@@ -5539,7 +5571,7 @@
   </sheetPr>
   <dimension ref="B1:M37"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A12" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="G37" sqref="G37"/>
     </sheetView>
   </sheetViews>
@@ -5568,7 +5600,7 @@
     </row>
     <row r="2" spans="2:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B2" s="95" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="3" spans="2:13" ht="15.6" x14ac:dyDescent="0.3">
@@ -5597,12 +5629,12 @@
     </row>
     <row r="33" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B33" s="3" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="34" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B34" s="4" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="35" spans="2:7" x14ac:dyDescent="0.25">
@@ -5619,10 +5651,10 @@
     </row>
     <row r="37" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B37" s="49" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="G37" s="28" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
   </sheetData>
@@ -5687,7 +5719,7 @@
     </row>
     <row r="2" spans="2:19" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B2" s="95" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
@@ -5712,7 +5744,7 @@
     </row>
     <row r="6" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B6" s="44" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C6" s="35" t="e">
         <f ca="1">CONCATENATE([0]!fy_max, calculation!$B$4)</f>
@@ -5721,7 +5753,7 @@
     </row>
     <row r="7" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B7" s="37" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C7" s="45" t="e">
         <f ca="1">VLOOKUP(CONCATENATE([0]!fy_max, "urban rural 6", $B7), [0]!data_range, 5, FALSE)</f>
@@ -5730,7 +5762,7 @@
     </row>
     <row r="8" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B8" s="39" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C8" s="46" t="e">
         <f ca="1">VLOOKUP(CONCATENATE([0]!fy_max, "urban rural 6", $B8), [0]!data_range, 5, FALSE)</f>
@@ -5739,7 +5771,7 @@
     </row>
     <row r="9" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B9" s="39" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C9" s="46" t="e">
         <f ca="1">VLOOKUP(CONCATENATE([0]!fy_max, "urban rural 6", $B9), [0]!data_range, 5, FALSE)</f>
@@ -5748,7 +5780,7 @@
     </row>
     <row r="10" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B10" s="39" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C10" s="46" t="e">
         <f ca="1">VLOOKUP(CONCATENATE([0]!fy_max, "urban rural 6", $B10), [0]!data_range, 5, FALSE)</f>
@@ -5757,7 +5789,7 @@
     </row>
     <row r="11" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B11" s="39" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C11" s="46" t="e">
         <f ca="1">VLOOKUP(CONCATENATE([0]!fy_max, "urban rural 6", $B11), [0]!data_range, 5, FALSE)</f>
@@ -5766,7 +5798,7 @@
     </row>
     <row r="12" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B12" s="41" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C12" s="47" t="e">
         <f ca="1">VLOOKUP(CONCATENATE([0]!fy_max, "urban rural 6", $B12), [0]!data_range, 5, FALSE)</f>
@@ -5798,7 +5830,7 @@
     </row>
     <row r="16" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B16" s="3" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C16" s="3"/>
       <c r="D16" s="3"/>
@@ -5810,7 +5842,7 @@
     </row>
     <row r="17" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B17" s="4" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C17" s="4"/>
       <c r="D17" s="4"/>
@@ -5834,10 +5866,10 @@
     </row>
     <row r="20" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B20" s="49" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D20" s="28" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
   </sheetData>
@@ -5888,7 +5920,7 @@
     </row>
     <row r="2" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B2" s="95" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="3" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
@@ -5914,12 +5946,12 @@
     </row>
     <row r="28" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B28" s="3" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="29" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B29" s="4" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="30" spans="2:6" x14ac:dyDescent="0.25">
@@ -5983,7 +6015,7 @@
     </row>
     <row r="2" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B2" s="95" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
@@ -6000,10 +6032,10 @@
         <v>79</v>
       </c>
       <c r="C6" s="35" t="s">
+        <v>137</v>
+      </c>
+      <c r="D6" s="50" t="s">
         <v>138</v>
-      </c>
-      <c r="D6" s="50" t="s">
-        <v>139</v>
       </c>
       <c r="E6" s="24"/>
       <c r="F6" s="24"/>
@@ -6244,12 +6276,12 @@
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B20" s="3" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B21" s="4" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.25">
@@ -6284,9 +6316,7 @@
   </sheetPr>
   <dimension ref="A2:AM164"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="C50" sqref="C50"/>
-    </sheetView>
+    <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
@@ -6873,10 +6903,10 @@
     </row>
     <row r="20" spans="1:3" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="25"/>
-      <c r="B20" s="109" t="s">
+      <c r="B20" s="108" t="s">
         <v>28</v>
       </c>
-      <c r="C20" s="109"/>
+      <c r="C20" s="108"/>
     </row>
     <row r="21" spans="1:3" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="25"/>
@@ -7024,15 +7054,15 @@
     </row>
     <row r="37" spans="1:3" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="25"/>
-      <c r="B37" s="110"/>
-      <c r="C37" s="110"/>
+      <c r="B37" s="109"/>
+      <c r="C37" s="109"/>
     </row>
     <row r="38" spans="1:3" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="25"/>
-      <c r="B38" s="109" t="s">
+      <c r="B38" s="108" t="s">
         <v>61</v>
       </c>
-      <c r="C38" s="109"/>
+      <c r="C38" s="108"/>
     </row>
     <row r="39" spans="1:3" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="25"/>
@@ -7076,7 +7106,7 @@
     <row r="44" spans="1:3" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="25"/>
       <c r="B44" s="12" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="45" spans="1:3" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -7091,7 +7121,7 @@
     <row r="47" spans="1:3" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="25"/>
       <c r="B47" s="5" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C47" s="2"/>
     </row>
@@ -7925,22 +7955,22 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="29" t="s">
+        <v>112</v>
+      </c>
+      <c r="B1" s="29" t="s">
         <v>113</v>
       </c>
-      <c r="B1" s="29" t="s">
+      <c r="C1" s="29" t="s">
         <v>114</v>
       </c>
-      <c r="C1" s="29" t="s">
+      <c r="D1" s="29" t="s">
         <v>115</v>
       </c>
-      <c r="D1" s="29" t="s">
+      <c r="E1" s="29" t="s">
         <v>116</v>
       </c>
-      <c r="E1" s="29" t="s">
+      <c r="F1" s="29" t="s">
         <v>117</v>
-      </c>
-      <c r="F1" s="29" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -30085,7 +30115,7 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="29" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B1" s="30">
         <f>COUNTA(data!B:B)-1</f>
@@ -30094,7 +30124,7 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="29" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B2" s="30">
         <f>COUNTA(data!1:1)</f>
@@ -30103,33 +30133,33 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="29" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B4" s="48" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="29" t="s">
+        <v>130</v>
+      </c>
+      <c r="B5" s="30" t="s">
         <v>131</v>
-      </c>
-      <c r="B5" s="30" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="29" t="s">
+        <v>149</v>
+      </c>
+      <c r="B6" s="89" t="s">
         <v>150</v>
-      </c>
-      <c r="B6" s="89" t="s">
-        <v>151</v>
       </c>
       <c r="I6" s="29"/>
       <c r="K6" s="29"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="29" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B7" s="30">
         <v>10</v>
@@ -30240,15 +30270,15 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="29" t="s">
+        <v>141</v>
+      </c>
+      <c r="B13" s="29" t="s">
         <v>142</v>
-      </c>
-      <c r="B13" s="29" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="29" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B14" s="30" t="e">
         <f ca="1">"Data for "&amp; $K$9 &amp;" are provisional. Please see Notes tab for more information."</f>
@@ -30257,34 +30287,34 @@
     </row>
     <row r="15" spans="1:11" ht="80.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="52" t="s">
-        <v>145</v>
-      </c>
-      <c r="B15" s="111" t="e">
+        <v>144</v>
+      </c>
+      <c r="B15" s="110" t="e">
         <f ca="1">IF($B$13 = "provisional", "Hospital data and ", "") &amp; "National Records of Scotland deaths data " &amp; IF($B$13 = "provisional", "are", "is") &amp; " provisional for " &amp; $K$9 &amp;". " &amp; IF($B$13 = "provisional", "This publication will be updated in October 20" &amp; RIGHT($K$9,2) &amp; ". " &amp; $B$16, "")</f>
         <v>#REF!</v>
       </c>
-      <c r="C15" s="111"/>
-      <c r="D15" s="111"/>
-      <c r="E15" s="111"/>
-      <c r="F15" s="111"/>
-      <c r="G15" s="111"/>
-      <c r="H15" s="111"/>
-      <c r="I15" s="111"/>
+      <c r="C15" s="110"/>
+      <c r="D15" s="110"/>
+      <c r="E15" s="110"/>
+      <c r="F15" s="110"/>
+      <c r="G15" s="110"/>
+      <c r="H15" s="110"/>
+      <c r="I15" s="110"/>
     </row>
     <row r="16" spans="1:11" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="29" t="s">
-        <v>146</v>
-      </c>
-      <c r="B16" s="112" t="s">
-        <v>162</v>
-      </c>
-      <c r="C16" s="111"/>
-      <c r="D16" s="111"/>
-      <c r="E16" s="111"/>
-      <c r="F16" s="111"/>
-      <c r="G16" s="111"/>
-      <c r="H16" s="111"/>
-      <c r="I16" s="111"/>
+        <v>145</v>
+      </c>
+      <c r="B16" s="111" t="s">
+        <v>161</v>
+      </c>
+      <c r="C16" s="110"/>
+      <c r="D16" s="110"/>
+      <c r="E16" s="110"/>
+      <c r="F16" s="110"/>
+      <c r="G16" s="110"/>
+      <c r="H16" s="110"/>
+      <c r="I16" s="110"/>
     </row>
     <row r="17" spans="1:9" ht="13.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="29"/>
@@ -30303,7 +30333,7 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="29" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B19" s="30" t="str">
         <f>"Figures in 2020/21 and 2021/22 are likely to have been affected by the impact of COVID-19 on hospital stays."</f>
@@ -30395,12 +30425,12 @@
     </row>
     <row r="30" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B30" s="3" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="31" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B31" s="4" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="32" spans="2:6" x14ac:dyDescent="0.25">
@@ -30733,12 +30763,12 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B21" s="3" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B22" s="4" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
@@ -30831,12 +30861,12 @@
     </row>
     <row r="36" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B36" s="3" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="37" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B37" s="4" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="38" spans="2:6" x14ac:dyDescent="0.25">
@@ -30853,12 +30883,12 @@
     </row>
     <row r="40" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B40" s="53" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="41" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B41" s="53" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
   </sheetData>
@@ -30921,7 +30951,7 @@
     </row>
     <row r="5" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B5" s="60" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C5" s="61" t="e">
         <f ca="1">CONCATENATE([0]!fy_max, calculation!$B$4)</f>
@@ -30936,7 +30966,7 @@
     </row>
     <row r="6" spans="2:11" ht="16.2" x14ac:dyDescent="0.25">
       <c r="B6" s="62" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C6" s="45" t="e">
         <f ca="1">VLOOKUP(CONCATENATE([0]!fy_max, "hb", $B6), [0]!data_range, 5, FALSE)</f>
@@ -30966,7 +30996,7 @@
     </row>
     <row r="8" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B8" s="48" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C8" s="46" t="e">
         <f ca="1">VLOOKUP(CONCATENATE([0]!fy_max, "hb", $B8), [0]!data_range, 5, FALSE)</f>
@@ -31028,7 +31058,7 @@
     </row>
     <row r="12" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B12" s="48" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C12" s="46" t="e">
         <f ca="1">VLOOKUP(CONCATENATE([0]!fy_max, "hb", $B12), [0]!data_range, 5, FALSE)</f>
@@ -31175,14 +31205,14 @@
     </row>
     <row r="23" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B23" s="3" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="J23" s="7"/>
       <c r="K23" s="7"/>
     </row>
     <row r="24" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B24" s="4" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="J24" s="7"/>
       <c r="K24" s="7"/>
@@ -31205,14 +31235,14 @@
     </row>
     <row r="27" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B27" s="53" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="J27" s="7"/>
       <c r="K27" s="7"/>
     </row>
     <row r="28" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B28" s="53" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="J28" s="7"/>
       <c r="K28" s="7"/>
@@ -31273,7 +31303,7 @@
   </sheetPr>
   <dimension ref="B1:M33"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="B12" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
@@ -31330,12 +31360,12 @@
     </row>
     <row r="30" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B30" s="3" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="31" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B31" s="4" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="32" spans="2:6" x14ac:dyDescent="0.25">
@@ -31369,10 +31399,10 @@
   <sheetPr codeName="Sheet7">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:Q27"/>
+  <dimension ref="B1:S27"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="M14" sqref="M14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -31383,7 +31413,7 @@
     <col min="4" max="16384" width="9.109375" style="56"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:19" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B1" s="104"/>
       <c r="C1" s="104"/>
       <c r="D1" s="104"/>
@@ -31397,18 +31427,18 @@
       <c r="L1" s="55"/>
       <c r="M1" s="55"/>
     </row>
-    <row r="2" spans="2:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:19" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B2" s="95" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="3" spans="2:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:19" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B3" s="95" t="e">
         <f ca="1" xml:space="preserve"> "by Age and Sex; " &amp; [0]!fy_max &amp; calculation!$B$4</f>
         <v>#REF!</v>
       </c>
     </row>
-    <row r="5" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:19" x14ac:dyDescent="0.25">
       <c r="J5" s="7"/>
       <c r="K5" s="7"/>
       <c r="L5" s="7"/>
@@ -31416,59 +31446,66 @@
       <c r="N5" s="7"/>
       <c r="O5" s="7"/>
     </row>
-    <row r="6" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B6" s="48"/>
-      <c r="C6" s="107" t="s">
+      <c r="C6" s="114" t="s">
         <v>100</v>
       </c>
-      <c r="D6" s="107"/>
-      <c r="E6" s="107"/>
-      <c r="F6" s="107"/>
-      <c r="G6" s="107"/>
-      <c r="H6" s="107"/>
-      <c r="J6" s="7"/>
+      <c r="D6" s="114"/>
+      <c r="E6" s="114"/>
+      <c r="F6" s="114"/>
+      <c r="G6" s="114"/>
+      <c r="H6" s="114"/>
+      <c r="I6" s="114"/>
+      <c r="J6" s="114"/>
       <c r="K6" s="7"/>
       <c r="Q6" s="58"/>
     </row>
-    <row r="7" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B7" s="82" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C7" s="83" t="s">
+        <v>177</v>
+      </c>
+      <c r="D7" s="83" t="s">
+        <v>176</v>
+      </c>
+      <c r="E7" s="83" t="s">
+        <v>175</v>
+      </c>
+      <c r="F7" s="83" t="s">
         <v>101</v>
       </c>
-      <c r="D7" s="83" t="s">
+      <c r="G7" s="83" t="s">
         <v>102</v>
       </c>
-      <c r="E7" s="83" t="s">
+      <c r="H7" s="83" t="s">
         <v>103</v>
       </c>
-      <c r="F7" s="83" t="s">
+      <c r="I7" s="83" t="s">
         <v>104</v>
       </c>
-      <c r="G7" s="83" t="s">
+      <c r="J7" s="83" t="s">
         <v>105</v>
       </c>
-      <c r="H7" s="83" t="s">
-        <v>106</v>
-      </c>
-      <c r="J7" s="7"/>
-      <c r="K7" s="7"/>
-      <c r="Q7" s="58"/>
-    </row>
-    <row r="8" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="L7" s="7"/>
+      <c r="M7" s="7"/>
+      <c r="S7" s="58"/>
+    </row>
+    <row r="8" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B8" s="48" t="s">
-        <v>130</v>
-      </c>
-      <c r="C8" s="46" t="e">
+        <v>129</v>
+      </c>
+      <c r="C8" s="112" t="e">
         <f ca="1">VLOOKUP(CONCATENATE([0]!fy_max, "age/sex", C$7, " ", $B8), [0]!data_range, 5, FALSE)</f>
         <v>#REF!</v>
       </c>
-      <c r="D8" s="46" t="e">
+      <c r="D8" s="112" t="e">
         <f ca="1">VLOOKUP(CONCATENATE([0]!fy_max, "age/sex", D$7, " ", $B8), [0]!data_range, 5, FALSE)</f>
         <v>#REF!</v>
       </c>
-      <c r="E8" s="46" t="e">
+      <c r="E8" s="112" t="e">
         <f ca="1">VLOOKUP(CONCATENATE([0]!fy_max, "age/sex", E$7, " ", $B8), [0]!data_range, 5, FALSE)</f>
         <v>#REF!</v>
       </c>
@@ -31484,19 +31521,27 @@
         <f ca="1">VLOOKUP(CONCATENATE([0]!fy_max, "age/sex", H$7, " ", $B8), [0]!data_range, 5, FALSE)</f>
         <v>#REF!</v>
       </c>
-      <c r="J8" s="7"/>
-      <c r="K8" s="7"/>
-      <c r="Q8" s="58"/>
-    </row>
-    <row r="9" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="I8" s="46" t="e">
+        <f ca="1">VLOOKUP(CONCATENATE([0]!fy_max, "age/sex", I$7, " ", $B8), [0]!data_range, 5, FALSE)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="J8" s="46" t="e">
+        <f ca="1">VLOOKUP(CONCATENATE([0]!fy_max, "age/sex", J$7, " ", $B8), [0]!data_range, 5, FALSE)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="L8" s="7"/>
+      <c r="M8" s="7"/>
+      <c r="S8" s="58"/>
+    </row>
+    <row r="9" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B9" s="48" t="s">
-        <v>107</v>
-      </c>
-      <c r="C9" s="46" t="e">
+        <v>106</v>
+      </c>
+      <c r="C9" s="112" t="e">
         <f ca="1">VLOOKUP(CONCATENATE([0]!fy_max, "age/sex", C$7, " ", $B9), [0]!data_range, 5, FALSE)</f>
         <v>#REF!</v>
       </c>
-      <c r="D9" s="46" t="e">
+      <c r="D9" s="112" t="e">
         <f ca="1">VLOOKUP(CONCATENATE([0]!fy_max, "age/sex", D$7, " ", $B9), [0]!data_range, 5, FALSE)</f>
         <v>#REF!</v>
       </c>
@@ -31516,19 +31561,27 @@
         <f ca="1">VLOOKUP(CONCATENATE([0]!fy_max, "age/sex", H$7, " ", $B9), [0]!data_range, 5, FALSE)</f>
         <v>#REF!</v>
       </c>
-      <c r="J9" s="58"/>
-      <c r="K9" s="58"/>
-      <c r="Q9" s="58"/>
-    </row>
-    <row r="10" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="I9" s="46" t="e">
+        <f ca="1">VLOOKUP(CONCATENATE([0]!fy_max, "age/sex", I$7, " ", $B9), [0]!data_range, 5, FALSE)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="J9" s="46" t="e">
+        <f ca="1">VLOOKUP(CONCATENATE([0]!fy_max, "age/sex", J$7, " ", $B9), [0]!data_range, 5, FALSE)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="L9" s="58"/>
+      <c r="M9" s="58"/>
+      <c r="S9" s="58"/>
+    </row>
+    <row r="10" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B10" s="84" t="s">
-        <v>108</v>
-      </c>
-      <c r="C10" s="47" t="e">
+        <v>107</v>
+      </c>
+      <c r="C10" s="113" t="e">
         <f ca="1">VLOOKUP(CONCATENATE([0]!fy_max, "age/sex", C$7, " ", $B10), [0]!data_range, 5, FALSE)</f>
         <v>#REF!</v>
       </c>
-      <c r="D10" s="47" t="e">
+      <c r="D10" s="113" t="e">
         <f ca="1">VLOOKUP(CONCATENATE([0]!fy_max, "age/sex", D$7, " ", $B10), [0]!data_range, 5, FALSE)</f>
         <v>#REF!</v>
       </c>
@@ -31548,15 +31601,23 @@
         <f ca="1">VLOOKUP(CONCATENATE([0]!fy_max, "age/sex", H$7, " ", $B10), [0]!data_range, 5, FALSE)</f>
         <v>#REF!</v>
       </c>
-      <c r="J10" s="58"/>
-      <c r="Q10" s="58"/>
-    </row>
-    <row r="11" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="I10" s="47" t="e">
+        <f ca="1">VLOOKUP(CONCATENATE([0]!fy_max, "age/sex", I$7, " ", $B10), [0]!data_range, 5, FALSE)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="J10" s="47" t="e">
+        <f ca="1">VLOOKUP(CONCATENATE([0]!fy_max, "age/sex", J$7, " ", $B10), [0]!data_range, 5, FALSE)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="L10" s="58"/>
+      <c r="S10" s="58"/>
+    </row>
+    <row r="11" spans="2:19" x14ac:dyDescent="0.25">
       <c r="J11" s="7"/>
       <c r="K11" s="7"/>
       <c r="Q11" s="58"/>
     </row>
-    <row r="12" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B12" s="2" t="s">
         <v>0</v>
       </c>
@@ -31567,29 +31628,29 @@
       <c r="K12" s="7"/>
       <c r="Q12" s="58"/>
     </row>
-    <row r="13" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B13" s="81"/>
       <c r="J13" s="7"/>
       <c r="K13" s="7"/>
       <c r="Q13" s="58"/>
     </row>
-    <row r="14" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B14" s="3" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="J14" s="7"/>
       <c r="K14" s="7"/>
       <c r="Q14" s="58"/>
     </row>
-    <row r="15" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B15" s="4" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="J15" s="7"/>
       <c r="K15" s="7"/>
       <c r="Q15" s="58"/>
     </row>
-    <row r="16" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B16" s="53" t="e">
         <f ca="1" xml:space="preserve"> "1. " &amp; calculation!$B$14</f>
         <v>#REF!</v>
@@ -31660,7 +31721,7 @@
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="B1:J1"/>
-    <mergeCell ref="C6:H6"/>
+    <mergeCell ref="C6:J6"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B12" location="'External Causes of Deaths'!A1" display="External causes of death excluded from analysis" xr:uid="{00000000-0004-0000-0600-000000000000}"/>
@@ -31678,7 +31739,7 @@
   </sheetPr>
   <dimension ref="B1:M42"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A12" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
@@ -31706,7 +31767,7 @@
     </row>
     <row r="2" spans="2:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B2" s="95" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="3" spans="2:13" ht="15.6" x14ac:dyDescent="0.3">
@@ -31739,7 +31800,7 @@
     </row>
     <row r="31" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B31" s="3" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C31" s="5"/>
       <c r="D31" s="5"/>
@@ -31748,7 +31809,7 @@
     </row>
     <row r="32" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B32" s="4" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C32" s="5"/>
       <c r="D32" s="5"/>
@@ -31768,27 +31829,27 @@
       </c>
     </row>
     <row r="35" spans="2:13" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="108" t="s">
-        <v>166</v>
-      </c>
-      <c r="C35" s="108"/>
-      <c r="D35" s="108"/>
-      <c r="E35" s="108"/>
-      <c r="F35" s="108"/>
-      <c r="G35" s="108"/>
-      <c r="H35" s="108"/>
-      <c r="I35" s="108"/>
-      <c r="J35" s="108"/>
-      <c r="K35" s="108"/>
-      <c r="L35" s="108"/>
-      <c r="M35" s="108"/>
+      <c r="B35" s="107" t="s">
+        <v>165</v>
+      </c>
+      <c r="C35" s="107"/>
+      <c r="D35" s="107"/>
+      <c r="E35" s="107"/>
+      <c r="F35" s="107"/>
+      <c r="G35" s="107"/>
+      <c r="H35" s="107"/>
+      <c r="I35" s="107"/>
+      <c r="J35" s="107"/>
+      <c r="K35" s="107"/>
+      <c r="L35" s="107"/>
+      <c r="M35" s="107"/>
     </row>
     <row r="36" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B36" s="49" t="s">
+        <v>108</v>
+      </c>
+      <c r="G36" s="28" t="s">
         <v>109</v>
-      </c>
-      <c r="G36" s="28" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="37" spans="2:13" x14ac:dyDescent="0.25">
@@ -31874,7 +31935,7 @@
     </row>
     <row r="2" spans="2:20" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B2" s="95" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
@@ -31907,7 +31968,7 @@
     </row>
     <row r="6" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B6" s="42" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C6" s="43" t="e">
         <f ca="1">CONCATENATE([0]!fy_max, calculation!$B$4)</f>
@@ -31922,7 +31983,7 @@
     </row>
     <row r="7" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B7" s="86" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C7" s="46" t="e">
         <f ca="1">VLOOKUP(CONCATENATE([0]!fy_max, "simd quintile", $B7), [0]!data_range, 5, FALSE)</f>
@@ -31982,7 +32043,7 @@
     </row>
     <row r="11" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B11" s="87" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C11" s="47" t="e">
         <f ca="1">VLOOKUP(CONCATENATE([0]!fy_max, "simd quintile", $B11), [0]!data_range, 5, FALSE)</f>
@@ -32030,7 +32091,7 @@
     </row>
     <row r="15" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B15" s="3" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C15" s="5"/>
       <c r="D15" s="5"/>
@@ -32039,7 +32100,7 @@
     </row>
     <row r="16" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B16" s="4" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C16" s="5"/>
       <c r="D16" s="5"/>
@@ -32059,27 +32120,27 @@
       </c>
     </row>
     <row r="19" spans="2:13" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="108" t="s">
-        <v>166</v>
-      </c>
-      <c r="C19" s="108"/>
-      <c r="D19" s="108"/>
-      <c r="E19" s="108"/>
-      <c r="F19" s="108"/>
-      <c r="G19" s="108"/>
-      <c r="H19" s="108"/>
-      <c r="I19" s="108"/>
-      <c r="J19" s="108"/>
-      <c r="K19" s="108"/>
-      <c r="L19" s="108"/>
-      <c r="M19" s="108"/>
+      <c r="B19" s="107" t="s">
+        <v>165</v>
+      </c>
+      <c r="C19" s="107"/>
+      <c r="D19" s="107"/>
+      <c r="E19" s="107"/>
+      <c r="F19" s="107"/>
+      <c r="G19" s="107"/>
+      <c r="H19" s="107"/>
+      <c r="I19" s="107"/>
+      <c r="J19" s="107"/>
+      <c r="K19" s="107"/>
+      <c r="L19" s="107"/>
+      <c r="M19" s="107"/>
     </row>
     <row r="20" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B20" s="49" t="s">
+        <v>108</v>
+      </c>
+      <c r="E20" s="28" t="s">
         <v>109</v>
-      </c>
-      <c r="E20" s="28" t="s">
-        <v>110</v>
       </c>
     </row>
   </sheetData>

</xml_diff>